<commit_message>
Fix, improve and refactor
</commit_message>
<xml_diff>
--- a/docs/source/_static/reports/prod/IFDAT-LIST.xlsx
+++ b/docs/source/_static/reports/prod/IFDAT-LIST.xlsx
@@ -16,9 +16,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ΠΕΡΙΕΧΟΜΕΝΑ'!$A$1:$A$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ΜΠΣ'!$A$1:$F$54</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'EO'!$A$1:$J$271</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ΕΚΔΟΣΕΙΣ ΜΕΤΟΧΩΝ ΕΟ'!$A$1:$D$362</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ΜΠΣ'!$A$1:$F$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'EO'!$A$1:$J$270</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'ΕΚΔΟΣΕΙΣ ΜΕΤΟΧΩΝ ΕΟ'!$A$1:$D$363</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'ΕΚΔΟΣΕΙΣ ΟΜΟΛΟΓΩΝ ΕΟ'!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1079,7 +1079,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B2" s="7" t="inlineStr">
         <is>
-          <t>L213800SHGGWDBFVRPS03, TGR094282521, BGR000920101000</t>
+          <t>TGR094282521, BGR000920101000, L213800SHGGWDBFVRPS03</t>
         </is>
       </c>
       <c r="C2" s="12" t="n">
@@ -1167,7 +1167,7 @@
       </c>
       <c r="B3" s="5" t="inlineStr">
         <is>
-          <t>L213800BEX8X28DTL5391, BGR000352001000, TGR094036844</t>
+          <t>L213800BEX8X28DTL5391, TGR094036844, BGR000352001000</t>
         </is>
       </c>
       <c r="C3" s="14" t="n">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B4" s="7" t="inlineStr">
         <is>
-          <t>L213800SMPWZVT6GGQZ69, TGR094493219, BGR002292401000</t>
+          <t>TGR094493219, L213800SMPWZVT6GGQZ69, BGR002292401000</t>
         </is>
       </c>
       <c r="C4" s="12" t="n">
@@ -1270,12 +1270,12 @@
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>EGRAK00003, EGRAK00014, EGRAK00124, EGRAK00125, EGRAK00136, EGRAK00139, EGRAK00215, EGRAK00219, EGRAK00253, EGRAK00270, EGRAK00401, EGRAK00428, EGRAK00450, EGRAK00469, EGRAK00512, EGRAK00560, EGRAK00823, EGRAK00828, EGRAK00848, EGRAK01004, EGRAK01006, EGRAK01014, EGRAK01018, EGRAK01028, EGRAK01044, EGRAK01048, EGRAK01053, EGRAK01077, EGRAK01078, EGRAK01089, EGRAK01091, EGRAK01096, EGRAK01101, EGRAK01113, EGRAK01117, EGRAK01122</t>
+          <t>EGRAK00003, EGRAK00014, EGRAK00124, EGRAK00125, EGRAK00136, EGRAK00139, EGRAK00215, EGRAK00219, EGRAK00253, EGRAK00270, EGRAK00401, EGRAK00428, EGRAK00450, EGRAK00469, EGRAK00512, EGRAK00560, EGRAK00823, EGRAK00828, EGRAK00848, EGRAK01004, EGRAK01006, EGRAK01014, EGRAK01018, EGRAK01028, EGRAK01044, EGRAK01048, EGRAK01053, EGRAK01077, EGRAK01078, EGRAK01089, EGRAK01091, EGRAK01096, EGRAK01101, EGRAK01113, EGRAK01117</t>
         </is>
       </c>
       <c r="F6" s="7" t="inlineStr">
         <is>
-          <t>EGRAK00003, EGRAK00014, EGRAK00124, EGRAK00125, EGRAK00136, EGRAK00139, EGRAK00215, EGRAK00219, EGRAK00253, EGRAK00270, EGRAK00401, EGRAK00428, EGRAK00450, EGRAK00469, EGRAK00512, EGRAK00560, EGRAK00823, EGRAK00828, EGRAK00848, EGRAK01004, EGRAK01006, EGRAK01014, EGRAK01018, EGRAK01028, EGRAK01044, EGRAK01048, EGRAK01053, EGRAK01077, EGRAK01078, EGRAK01089, EGRAK01091, EGRAK01096, EGRAK01101, EGRAK01113, EGRAK01117, EGRAK01122</t>
+          <t>EGRAK00003, EGRAK00014, EGRAK00124, EGRAK00125, EGRAK00136, EGRAK00139, EGRAK00215, EGRAK00219, EGRAK00253, EGRAK00270, EGRAK00401, EGRAK00428, EGRAK00450, EGRAK00469, EGRAK00512, EGRAK00560, EGRAK00823, EGRAK00828, EGRAK00848, EGRAK01004, EGRAK01006, EGRAK01014, EGRAK01018, EGRAK01028, EGRAK01044, EGRAK01048, EGRAK01053, EGRAK01077, EGRAK01078, EGRAK01089, EGRAK01091, EGRAK01096, EGRAK01101, EGRAK01113, EGRAK01117</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>BGR001003501000, TGR094304867, L213800UWXVWAKFGVLB36</t>
+          <t>TGR094304867, BGR001003501000, L213800UWXVWAKFGVLB36</t>
         </is>
       </c>
       <c r="C7" s="14" t="n">
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>L213800U6WAX3YXMFVH22, TGR094354938, BGR000942001000</t>
+          <t>TGR094354938, L213800U6WAX3YXMFVH22, BGR000942001000</t>
         </is>
       </c>
       <c r="C8" s="12" t="n">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>BGR000832401000, TGR094325107, L213800YSZHWSCLXXRI37</t>
+          <t>L213800YSZHWSCLXXRI37, TGR094325107, BGR000832401000</t>
         </is>
       </c>
       <c r="C9" s="14" t="n">
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>BGR000918601000, L635400S5G5WWGN6B8T87, TGR094351475</t>
+          <t>TGR094351475, BGR000918601000, L635400S5G5WWGN6B8T87</t>
         </is>
       </c>
       <c r="C10" s="12" t="n">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>L213800XXMES8I6GQVQ47, TGR099553209, BGR003581901000</t>
+          <t>TGR099553209, BGR003581901000, L213800XXMES8I6GQVQ47</t>
         </is>
       </c>
       <c r="C11" s="14" t="n">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B12" s="7" t="inlineStr">
         <is>
-          <t>L549300JSLNCWDXJT4U81, BGR003931601000, TGR099760120</t>
+          <t>TGR099760120, L549300JSLNCWDXJT4U81, BGR003931601000</t>
         </is>
       </c>
       <c r="C12" s="12" t="n">
@@ -1462,1225 +1462,1255 @@
     <row r="13" ht="36" customHeight="1">
       <c r="A13" s="13" t="inlineStr">
         <is>
-          <t>EGRAEEX002</t>
+          <t>EGR099757323</t>
         </is>
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>TGR099759863, BGR003882701000, L213800USGL7Q5UR9M221</t>
+          <t>BGR122032001000, L9845003A94A6F41EB779, TGR099757323</t>
         </is>
       </c>
       <c r="C13" s="14" t="n">
-        <v>36732</v>
+        <v>36656</v>
       </c>
       <c r="D13" s="5" t="inlineStr">
         <is>
-          <t>ALPHA TRUST- ΑΝΔΡΟΜΕΔΑ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΧΑΡΤΟΦΥΛΑΚΙΟΥ</t>
-        </is>
-      </c>
-      <c r="E13" s="5" t="inlineStr"/>
+          <t>ELIKONOS CAPITAL ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΟΡΓΑΝΙΣΜΩΝ ΕΝΑΛΛΑΚΤΙΚΩΝ ΕΠΕΝΔΥΣΕΩΝ</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t>EGRAK01057</t>
+        </is>
+      </c>
       <c r="F13" s="5" t="inlineStr">
         <is>
-          <t>EGRAEEX002</t>
+          <t>EGRAK01057</t>
         </is>
       </c>
     </row>
     <row r="14" ht="36" customHeight="1">
       <c r="A14" s="11" t="inlineStr">
         <is>
-          <t>EGR999984680</t>
+          <t>EGRAEEX002</t>
         </is>
       </c>
       <c r="B14" s="7" t="inlineStr">
         <is>
-          <t>L984500EE5E3BA3F08B21, TGR999984680, BGR004373001000</t>
+          <t>BGR003882701000, L213800USGL7Q5UR9M221, TGR099759863</t>
         </is>
       </c>
       <c r="C14" s="12" t="n">
-        <v>37069</v>
+        <v>36732</v>
       </c>
       <c r="D14" s="7" t="inlineStr">
         <is>
-          <t>ΕΛΛΕΝΙΚ ΚΑΠΙΤΑΛ ΠΑΡΤΝΕΡΣ ΑΝΩΝΥΜΟΣ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΕΩΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
-        </is>
-      </c>
-      <c r="E14" s="7" t="inlineStr">
-        <is>
-          <t>EGRAK01061, EGRAK01068</t>
-        </is>
-      </c>
+          <t>ALPHA TRUST- ΑΝΔΡΟΜΕΔΑ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΧΑΡΤΟΦΥΛΑΚΙΟΥ</t>
+        </is>
+      </c>
+      <c r="E14" s="7" t="inlineStr"/>
       <c r="F14" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01061, EGRAK01068</t>
+          <t>EGRAEEX002</t>
         </is>
       </c>
     </row>
     <row r="15" ht="36" customHeight="1">
       <c r="A15" s="13" t="inlineStr">
         <is>
-          <t>EGRAEEAP002</t>
+          <t>EGR999984680</t>
         </is>
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>TGR099554901, L213800U7SBKWW79CBG88, BGR003548801000</t>
+          <t>BGR004373001000, L984500EE5E3BA3F08B21, TGR999984680</t>
         </is>
       </c>
       <c r="C15" s="14" t="n">
-        <v>37711</v>
+        <v>37069</v>
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>TRASTOR ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΑΚΙΝΗΤΗΣ ΠΕΡΙΟΥΣΙΑΣ</t>
-        </is>
-      </c>
-      <c r="E15" s="5" t="inlineStr"/>
+          <t>ΕΛΛΕΝΙΚ ΚΑΠΙΤΑΛ ΠΑΡΤΝΕΡΣ ΑΝΩΝΥΜΟΣ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΕΩΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr">
+        <is>
+          <t>EGRAK01061, EGRAK01068</t>
+        </is>
+      </c>
       <c r="F15" s="5" t="inlineStr">
         <is>
-          <t>EGRAEEAP002</t>
+          <t>EGRAK01061, EGRAK01068</t>
         </is>
       </c>
     </row>
     <row r="16" ht="36" customHeight="1">
       <c r="A16" s="11" t="inlineStr">
         <is>
-          <t>EGRAEPEY059</t>
+          <t>EGRAEEAP002</t>
         </is>
       </c>
       <c r="B16" s="7" t="inlineStr">
         <is>
-          <t>L213800P8QPUPE3SOGX14, BGR006816701000, TGR998940936</t>
+          <t>TGR099554901, L213800U7SBKWW79CBG88, BGR003548801000</t>
         </is>
       </c>
       <c r="C16" s="12" t="n">
-        <v>38776</v>
+        <v>37711</v>
       </c>
       <c r="D16" s="7" t="inlineStr">
         <is>
-          <t>THETIS CAPITAL ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΠΑΡΟΧΗΣ ΕΠΕΝΔΥΤΙΚΩΝ ΥΠΗΡΕΣΙΩΝ</t>
-        </is>
-      </c>
-      <c r="E16" s="7" t="inlineStr">
-        <is>
-          <t>EGRAK90012</t>
-        </is>
-      </c>
+          <t>TRASTOR ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΑΚΙΝΗΤΗΣ ΠΕΡΙΟΥΣΙΑΣ</t>
+        </is>
+      </c>
+      <c r="E16" s="7" t="inlineStr"/>
       <c r="F16" s="7" t="inlineStr">
         <is>
-          <t>EGRAK90012</t>
+          <t>EGRAEEAP002</t>
         </is>
       </c>
     </row>
     <row r="17" ht="36" customHeight="1">
       <c r="A17" s="13" t="inlineStr">
         <is>
-          <t>EGR998642355</t>
+          <t>EGRAEPEY059</t>
         </is>
       </c>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>L2138001MKHE9G2UERJ13, TGR998642355, BGR007175901000</t>
+          <t>TGR998940936, BGR006816701000, L213800P8QPUPE3SOGX14</t>
         </is>
       </c>
       <c r="C17" s="14" t="n">
-        <v>39024</v>
+        <v>38776</v>
       </c>
       <c r="D17" s="5" t="inlineStr">
         <is>
-          <t>CNL ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΟΡΓΑΝΙΣΜΩΝ ΕΝΑΛΛΑΚΤΙΚΩΝ ΕΠΕΝΔΥΣΕΩΝ</t>
+          <t>THETIS CAPITAL ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΠΑΡΟΧΗΣ ΕΠΕΝΔΥΤΙΚΩΝ ΥΠΗΡΕΣΙΩΝ</t>
         </is>
       </c>
       <c r="E17" s="5" t="inlineStr">
         <is>
-          <t>EGREKES001</t>
+          <t>EGRAK90012</t>
         </is>
       </c>
       <c r="F17" s="5" t="inlineStr">
         <is>
-          <t>EGREKES001</t>
+          <t>EGRAK90012</t>
         </is>
       </c>
     </row>
     <row r="18" ht="36" customHeight="1">
       <c r="A18" s="11" t="inlineStr">
         <is>
-          <t>EGRAEEAP003</t>
+          <t>EGR998642355</t>
         </is>
       </c>
       <c r="B18" s="7" t="inlineStr">
         <is>
-          <t>TGR099555020, BGR003546201000, L549300XDXYOF57JOFT72</t>
+          <t>L2138001MKHE9G2UERJ13, TGR998642355, BGR007175901000</t>
         </is>
       </c>
       <c r="C18" s="12" t="n">
-        <v>39321</v>
+        <v>39024</v>
       </c>
       <c r="D18" s="7" t="inlineStr">
         <is>
-          <t>Προντέα Ανώνυμη Εταιρεία Επενδύσεων σε Ακίνητη Περιουσία</t>
-        </is>
-      </c>
-      <c r="E18" s="7" t="inlineStr"/>
+          <t>CNL ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΟΡΓΑΝΙΣΜΩΝ ΕΝΑΛΛΑΚΤΙΚΩΝ ΕΠΕΝΔΥΣΕΩΝ</t>
+        </is>
+      </c>
+      <c r="E18" s="7" t="inlineStr">
+        <is>
+          <t>EGREKES001</t>
+        </is>
+      </c>
       <c r="F18" s="7" t="inlineStr">
         <is>
-          <t>EGRAEEAP003</t>
+          <t>EGREKES001</t>
         </is>
       </c>
     </row>
     <row r="19" ht="36" customHeight="1">
       <c r="A19" s="13" t="inlineStr">
         <is>
-          <t>EGR998279015</t>
+          <t>EGRAEEAP003</t>
         </is>
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>TGR998279015, BGR007914601000</t>
+          <t>TGR099555020, BGR003546201000, L549300XDXYOF57JOFT72</t>
         </is>
       </c>
       <c r="C19" s="14" t="n">
-        <v>39407</v>
+        <v>39321</v>
       </c>
       <c r="D19" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS CAPITAL MANAGEMENT ΑΜΟΙΒΑΙΑ ΚΕΦΑΛΑΙΑ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ ΜΟΝΟΠΡΟΣΩΠΗ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ</t>
-        </is>
-      </c>
-      <c r="E19" s="5" t="inlineStr">
-        <is>
-          <t>EGRAK90005</t>
-        </is>
-      </c>
+          <t>Προντέα Ανώνυμη Εταιρεία Επενδύσεων σε Ακίνητη Περιουσία</t>
+        </is>
+      </c>
+      <c r="E19" s="5" t="inlineStr"/>
       <c r="F19" s="5" t="inlineStr">
         <is>
-          <t>EGRAK90005</t>
+          <t>EGRAEEAP003</t>
         </is>
       </c>
     </row>
     <row r="20" ht="36" customHeight="1">
       <c r="A20" s="11" t="inlineStr">
         <is>
-          <t>EGR998159392</t>
+          <t>EGR998279015</t>
         </is>
       </c>
       <c r="B20" s="7" t="inlineStr">
         <is>
-          <t>L213800ESHXNWYJAEMO70, BGR008234001000, TGR998159392</t>
+          <t>TGR998279015, BGR007914601000</t>
         </is>
       </c>
       <c r="C20" s="12" t="n">
-        <v>39942</v>
+        <v>39407</v>
       </c>
       <c r="D20" s="7" t="inlineStr">
         <is>
-          <t>ΑΛΦΑ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ - ΑΚΕΣ</t>
+          <t>PIRAEUS CAPITAL MANAGEMENT ΑΜΟΙΒΑΙΑ ΚΕΦΑΛΑΙΑ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ ΜΟΝΟΠΡΟΣΩΠΗ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ</t>
         </is>
       </c>
       <c r="E20" s="7" t="inlineStr">
         <is>
-          <t>EGRAK90014</t>
+          <t>EGRAK90005</t>
         </is>
       </c>
       <c r="F20" s="7" t="inlineStr">
         <is>
-          <t>EGRAK90014</t>
+          <t>EGRAK90005</t>
         </is>
       </c>
     </row>
     <row r="21" ht="36" customHeight="1">
       <c r="A21" s="13" t="inlineStr">
         <is>
-          <t>EGR800398384</t>
+          <t>EGR998159392</t>
         </is>
       </c>
       <c r="B21" s="5" t="inlineStr">
         <is>
-          <t>L21380099L8WQI3DI3Y74, BGR120129501000, TGR800398384</t>
+          <t>BGR008234001000, L213800ESHXNWYJAEMO70, TGR998159392</t>
         </is>
       </c>
       <c r="C21" s="14" t="n">
-        <v>40992</v>
+        <v>39942</v>
       </c>
       <c r="D21" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS JEREMIE TECHNOLOGY CATALYST MANAGEMENT ΜΟΝΟΠΡΟΣΩΠΗ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>ΑΛΦΑ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ - ΑΚΕΣ</t>
         </is>
       </c>
       <c r="E21" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01057, EGRAK90007</t>
+          <t>EGRAK90014</t>
         </is>
       </c>
       <c r="F21" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01057, EGRAK90007</t>
+          <t>EGRAK90014</t>
         </is>
       </c>
     </row>
     <row r="22" ht="36" customHeight="1">
       <c r="A22" s="11" t="inlineStr">
         <is>
-          <t>EGR800433747</t>
+          <t>EGR800398384</t>
         </is>
       </c>
       <c r="B22" s="7" t="inlineStr">
         <is>
-          <t>TGR800433747, L2138006SQBPKYG6GZX87, BGR122339001000</t>
+          <t>L21380099L8WQI3DI3Y74, BGR120129501000, TGR800398384</t>
         </is>
       </c>
       <c r="C22" s="12" t="n">
-        <v>41162</v>
+        <v>40992</v>
       </c>
       <c r="D22" s="7" t="inlineStr">
         <is>
-          <t>Openfund Ανώνυμη Εταιρία Διαχείρισης Αμοιβαίων Κεφαλαίων Επιχειρηματικών Συμμετοχών</t>
+          <t>PIRAEUS JEREMIE TECHNOLOGY CATALYST MANAGEMENT ΜΟΝΟΠΡΟΣΩΠΗ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E22" s="7" t="inlineStr">
         <is>
-          <t>EGRAK90006</t>
+          <t>EGRAK90007</t>
         </is>
       </c>
       <c r="F22" s="7" t="inlineStr">
         <is>
-          <t>EGRAK90006</t>
+          <t>EGRAK90007</t>
         </is>
       </c>
     </row>
     <row r="23" ht="36" customHeight="1">
       <c r="A23" s="13" t="inlineStr">
         <is>
-          <t>EGRAEEAP007</t>
+          <t>EGR800433747</t>
         </is>
       </c>
       <c r="B23" s="5" t="inlineStr">
         <is>
-          <t>TGR997656128, L213800Q23BDHSW1OQT90, BGR128686346000</t>
+          <t>BGR122339001000, TGR800433747, L2138006SQBPKYG6GZX87</t>
         </is>
       </c>
       <c r="C23" s="14" t="n">
-        <v>41657</v>
+        <v>41162</v>
       </c>
       <c r="D23" s="5" t="inlineStr">
         <is>
-          <t>ΜΠΛΕ ΚΕΔΡΟΣ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΑΚΙΝΗΤΗΣ ΠΕΡΙΟΥΣΙΑΣ</t>
-        </is>
-      </c>
-      <c r="E23" s="5" t="inlineStr"/>
+          <t>Openfund Ανώνυμη Εταιρία Διαχείρισης Αμοιβαίων Κεφαλαίων Επιχειρηματικών Συμμετοχών</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="inlineStr">
+        <is>
+          <t>EGRAK90006</t>
+        </is>
+      </c>
       <c r="F23" s="5" t="inlineStr">
         <is>
-          <t>EGRAEEAP007</t>
+          <t>EGRAK90006</t>
         </is>
       </c>
     </row>
     <row r="24" ht="36" customHeight="1">
       <c r="A24" s="11" t="inlineStr">
         <is>
-          <t>EGRAEEAP006</t>
+          <t>EGRAEEAP007</t>
         </is>
       </c>
       <c r="B24" s="7" t="inlineStr">
         <is>
-          <t>L213800TBZBVWRUAOPV78, BGR140330201000, TGR997521479</t>
+          <t>TGR997656128, BGR128686346000, L213800Q23BDHSW1OQT90</t>
         </is>
       </c>
       <c r="C24" s="12" t="n">
-        <v>42664</v>
+        <v>41657</v>
       </c>
       <c r="D24" s="7" t="inlineStr">
         <is>
-          <t>BriQ Properties Ανώνυμη Εταιρεία Επενδύσεων σε Ακίνητη Περιουσία</t>
+          <t>ΜΠΛΕ ΚΕΔΡΟΣ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΑΚΙΝΗΤΗΣ ΠΕΡΙΟΥΣΙΑΣ</t>
         </is>
       </c>
       <c r="E24" s="7" t="inlineStr"/>
       <c r="F24" s="7" t="inlineStr">
         <is>
-          <t>EGRAEEAP006</t>
+          <t>EGRAEEAP007</t>
         </is>
       </c>
     </row>
     <row r="25" ht="36" customHeight="1">
       <c r="A25" s="13" t="inlineStr">
         <is>
-          <t>EGR800792234</t>
+          <t>EGRAEEAP006</t>
         </is>
       </c>
       <c r="B25" s="5" t="inlineStr">
         <is>
-          <t>TGR800792234, BGR141064201000, L213800PZN3W777G7XR07</t>
+          <t>L213800TBZBVWRUAOPV78, BGR140330201000, TGR997521479</t>
         </is>
       </c>
       <c r="C25" s="14" t="n">
-        <v>42744</v>
+        <v>42664</v>
       </c>
       <c r="D25" s="5" t="inlineStr">
         <is>
-          <t>Marathon Ανώνυμη Εταιρία Διαχείρισης Αμοιβαίων Κεφαλαίων Επιχειρηματικών Συμμετοχών</t>
-        </is>
-      </c>
-      <c r="E25" s="5" t="inlineStr">
-        <is>
-          <t>EGRAK01062, EGRAK01063</t>
-        </is>
-      </c>
+          <t>BriQ Properties Ανώνυμη Εταιρεία Επενδύσεων σε Ακίνητη Περιουσία</t>
+        </is>
+      </c>
+      <c r="E25" s="5" t="inlineStr"/>
       <c r="F25" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01062, EGRAK01063</t>
+          <t>EGRAEEAP006</t>
         </is>
       </c>
     </row>
     <row r="26" ht="36" customHeight="1">
       <c r="A26" s="11" t="inlineStr">
         <is>
-          <t>EGRMFMC030</t>
+          <t>EGR800792234</t>
         </is>
       </c>
       <c r="B26" s="7" t="inlineStr">
         <is>
-          <t>BGR142754460000, TGR997010182, L254900CCGB73PBHKXL72</t>
+          <t>L213800PZN3W777G7XR07, TGR800792234, BGR141064201000</t>
         </is>
       </c>
       <c r="C26" s="12" t="n">
-        <v>42887</v>
+        <v>42744</v>
       </c>
       <c r="D26" s="7" t="inlineStr">
         <is>
-          <t>ATHOS ASSET MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ</t>
+          <t>Marathon Ανώνυμη Εταιρία Διαχείρισης Αμοιβαίων Κεφαλαίων Επιχειρηματικών Συμμετοχών</t>
         </is>
       </c>
       <c r="E26" s="7" t="inlineStr">
         <is>
-          <t>EGRAK00238, EGRAK00465, EGRAK00552, EGRAK00553, EGRAK00554, EGRAK00555, EGRAK00592, EGRAK00835, EGRAK00854, EGRAK01112</t>
+          <t>EGRAK01062, EGRAK01063</t>
         </is>
       </c>
       <c r="F26" s="7" t="inlineStr">
         <is>
-          <t>EGRAK00238, EGRAK00465, EGRAK00552, EGRAK00553, EGRAK00554, EGRAK00555, EGRAK00592, EGRAK00835, EGRAK00854, EGRAK01112</t>
+          <t>EGRAK01062, EGRAK01063</t>
         </is>
       </c>
     </row>
     <row r="27" ht="36" customHeight="1">
       <c r="A27" s="13" t="inlineStr">
         <is>
-          <t>EGR800903737</t>
+          <t>EGRMFMC030</t>
         </is>
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>TGR800903737, L9845007DB3RB2B4DN624, BGR144560003000</t>
+          <t>L254900CCGB73PBHKXL72, TGR997010182, BGR142754460000</t>
         </is>
       </c>
       <c r="C27" s="14" t="n">
-        <v>43074</v>
+        <v>42887</v>
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>METAVALLON PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>ATHOS ASSET MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01064, EGRAK01065</t>
+          <t>EGRAK00238, EGRAK00465, EGRAK00552, EGRAK00553, EGRAK00554, EGRAK00555, EGRAK00592, EGRAK00835, EGRAK00854, EGRAK01112</t>
         </is>
       </c>
       <c r="F27" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01064, EGRAK01065</t>
+          <t>EGRAK00238, EGRAK00465, EGRAK00552, EGRAK00553, EGRAK00554, EGRAK00555, EGRAK00592, EGRAK00835, EGRAK00854, EGRAK01112</t>
         </is>
       </c>
     </row>
     <row r="28" ht="36" customHeight="1">
       <c r="A28" s="11" t="inlineStr">
         <is>
-          <t>EGR800911079</t>
+          <t>EGR800903737</t>
         </is>
       </c>
       <c r="B28" s="7" t="inlineStr">
         <is>
-          <t>BGR144725001000, TGR800911079</t>
+          <t>L9845007DB3RB2B4DN624, TGR800903737, BGR144560003000</t>
         </is>
       </c>
       <c r="C28" s="12" t="n">
-        <v>43090</v>
+        <v>43074</v>
       </c>
       <c r="D28" s="7" t="inlineStr">
         <is>
-          <t>ΓΙΟΥΝΙΦΑΝΤ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>METAVALLON PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E28" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01070, EGRAK01071</t>
+          <t>EGRAK01064, EGRAK01065</t>
         </is>
       </c>
       <c r="F28" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01070, EGRAK01071</t>
+          <t>EGRAK01064, EGRAK01065</t>
         </is>
       </c>
     </row>
     <row r="29" ht="36" customHeight="1">
       <c r="A29" s="13" t="inlineStr">
         <is>
-          <t>EGRAEEAP008</t>
+          <t>EGR800911079</t>
         </is>
       </c>
       <c r="B29" s="5" t="inlineStr">
         <is>
-          <t>L213800DTEZE6R8BZ9K19, BGR148547901000, TGR801077433</t>
+          <t>BGR144725001000, TGR800911079</t>
         </is>
       </c>
       <c r="C29" s="14" t="n">
-        <v>43448</v>
+        <v>43090</v>
       </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
-          <t>ORILINA PROPERTIES ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΕΠΕΝΔΥΣΕΩΝ ΣΕ ΑΚΙΝΗΤΗ ΠΕΡΙΟΥΣΙΑ</t>
-        </is>
-      </c>
-      <c r="E29" s="5" t="inlineStr"/>
+          <t>ΓΙΟΥΝΙΦΑΝΤ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+        </is>
+      </c>
+      <c r="E29" s="5" t="inlineStr">
+        <is>
+          <t>EGRAK01070, EGRAK01071</t>
+        </is>
+      </c>
       <c r="F29" s="5" t="inlineStr">
         <is>
-          <t>EGRAEEAP008</t>
+          <t>EGRAK01070, EGRAK01071</t>
         </is>
       </c>
     </row>
     <row r="30" ht="36" customHeight="1">
       <c r="A30" s="11" t="inlineStr">
         <is>
-          <t>EGRAEEAP010</t>
+          <t>EGRAEEAP008</t>
         </is>
       </c>
       <c r="B30" s="7" t="inlineStr">
         <is>
-          <t>TGR996899546, L213800XKY8GHKN57D970, BGR152321260000</t>
+          <t>BGR148547901000, L213800DTEZE6R8BZ9K19, TGR801077433</t>
         </is>
       </c>
       <c r="C30" s="12" t="n">
-        <v>43752</v>
+        <v>43448</v>
       </c>
       <c r="D30" s="7" t="inlineStr">
         <is>
-          <t>ΝΟΒΑΛ ΠΡΟΠΕΡΤΥ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΣΕ ΑΚΙΝΗΤΗ ΠΕΡΙΟΥΣΙΑ</t>
+          <t>ORILINA PROPERTIES ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΕΠΕΝΔΥΣΕΩΝ ΣΕ ΑΚΙΝΗΤΗ ΠΕΡΙΟΥΣΙΑ</t>
         </is>
       </c>
       <c r="E30" s="7" t="inlineStr"/>
       <c r="F30" s="7" t="inlineStr">
         <is>
-          <t>EGRAEEAP010</t>
+          <t>EGRAEEAP008</t>
         </is>
       </c>
     </row>
     <row r="31" ht="36" customHeight="1">
       <c r="A31" s="13" t="inlineStr">
         <is>
-          <t>EGR801296864</t>
+          <t>EGRAEEAP010</t>
         </is>
       </c>
       <c r="B31" s="5" t="inlineStr">
         <is>
-          <t>TGR801296814, BGR153787304000, L9845007855485B71CC46</t>
+          <t>L213800XKY8GHKN57D970, BGR152321260000, TGR996899546</t>
         </is>
       </c>
       <c r="C31" s="14" t="n">
-        <v>43864</v>
+        <v>43752</v>
       </c>
       <c r="D31" s="5" t="inlineStr">
         <is>
-          <t>THERMI VENTURE CAPITAL MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
-        </is>
-      </c>
-      <c r="E31" s="5" t="inlineStr">
-        <is>
-          <t>EGRAK01027</t>
-        </is>
-      </c>
+          <t>ΝΟΒΑΛ ΠΡΟΠΕΡΤΥ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΣΕ ΑΚΙΝΗΤΗ ΠΕΡΙΟΥΣΙΑ</t>
+        </is>
+      </c>
+      <c r="E31" s="5" t="inlineStr"/>
       <c r="F31" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01027</t>
+          <t>EGRAEEAP010</t>
         </is>
       </c>
     </row>
     <row r="32" ht="36" customHeight="1">
       <c r="A32" s="11" t="inlineStr">
         <is>
-          <t>EGR801322351</t>
+          <t>EGR801296864</t>
         </is>
       </c>
       <c r="B32" s="7" t="inlineStr">
         <is>
-          <t>TGR801322351, BGR154382104000</t>
+          <t>BGR153787304000, L9845007855485B71CC46, TGR801296814</t>
         </is>
       </c>
       <c r="C32" s="12" t="n">
-        <v>43896</v>
+        <v>43864</v>
       </c>
       <c r="D32" s="7" t="inlineStr">
         <is>
-          <t>VENTURE STORIES PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>THERMI VENTURE CAPITAL MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E32" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01069</t>
+          <t>EGRAK01027</t>
         </is>
       </c>
       <c r="F32" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01069</t>
+          <t>EGRAK01027</t>
         </is>
       </c>
     </row>
     <row r="33" ht="36" customHeight="1">
       <c r="A33" s="13" t="inlineStr">
         <is>
-          <t>EGR801446716</t>
+          <t>EGR801322351</t>
         </is>
       </c>
       <c r="B33" s="5" t="inlineStr">
         <is>
-          <t>BGR157033507000, TGR801446716, L9845003A111B06B9D568</t>
+          <t>TGR801322351, BGR154382104000</t>
         </is>
       </c>
       <c r="C33" s="14" t="n">
-        <v>44141</v>
+        <v>43896</v>
       </c>
       <c r="D33" s="5" t="inlineStr">
         <is>
-          <t>ROCHELLE CAPITAL MANAGEMENT ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ</t>
+          <t>VENTURE STORIES PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E33" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01058</t>
+          <t>EGRAK01069</t>
         </is>
       </c>
       <c r="F33" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01058</t>
+          <t>EGRAK01069</t>
         </is>
       </c>
     </row>
     <row r="34" ht="36" customHeight="1">
       <c r="A34" s="11" t="inlineStr">
         <is>
-          <t>EGR801446949</t>
+          <t>EGR801446716</t>
         </is>
       </c>
       <c r="B34" s="7" t="inlineStr">
         <is>
-          <t>L9845004F1F377E786787, TGR801446949, BGR157036301000</t>
+          <t>TGR801446716, BGR157033507000, L9845003A111B06B9D568</t>
         </is>
       </c>
       <c r="C34" s="12" t="n">
-        <v>44142</v>
+        <v>44141</v>
       </c>
       <c r="D34" s="7" t="inlineStr">
         <is>
-          <t>GREEK BRANDS VENTURES ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ - ΑΕΔΑΚΕΣ</t>
+          <t>ROCHELLE CAPITAL MANAGEMENT ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ</t>
         </is>
       </c>
       <c r="E34" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01060</t>
+          <t>EGRAK01058</t>
         </is>
       </c>
       <c r="F34" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01060</t>
+          <t>EGRAK01058</t>
         </is>
       </c>
     </row>
     <row r="35" ht="36" customHeight="1">
       <c r="A35" s="13" t="inlineStr">
         <is>
-          <t>EGR801470046</t>
+          <t>EGR801446949</t>
         </is>
       </c>
       <c r="B35" s="5" t="inlineStr">
         <is>
-          <t>TGR801470046, BGR157511601000, L2138006VXU6UDW7P6H67</t>
+          <t>TGR801446949, BGR157036301000, L9845004F1F377E786787</t>
         </is>
       </c>
       <c r="C35" s="14" t="n">
-        <v>44179</v>
+        <v>44142</v>
       </c>
       <c r="D35" s="5" t="inlineStr">
         <is>
-          <t>NEW ENERGY PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>GREEK BRANDS VENTURES ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ - ΑΕΔΑΚΕΣ</t>
         </is>
       </c>
       <c r="E35" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01066</t>
+          <t>EGRAK01060</t>
         </is>
       </c>
       <c r="F35" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01066</t>
+          <t>EGRAK01060</t>
         </is>
       </c>
     </row>
     <row r="36" ht="36" customHeight="1">
       <c r="A36" s="11" t="inlineStr">
         <is>
-          <t>EGR996764210</t>
+          <t>EGR801470046</t>
         </is>
       </c>
       <c r="B36" s="7" t="inlineStr">
         <is>
-          <t>TGR996764210, BGR157802360000</t>
+          <t>BGR157511601000, TGR801470046, L2138006VXU6UDW7P6H67</t>
         </is>
       </c>
       <c r="C36" s="12" t="n">
-        <v>44210</v>
+        <v>44179</v>
       </c>
       <c r="D36" s="7" t="inlineStr">
         <is>
-          <t>ΣΥΜΜΕΤΟΧΕΣ 5G Ανώνυμη Εταιρεία</t>
+          <t>NEW ENERGY PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E36" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01067</t>
+          <t>EGRAK01066</t>
         </is>
       </c>
       <c r="F36" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01067</t>
+          <t>EGRAK01066</t>
         </is>
       </c>
     </row>
     <row r="37" ht="36" customHeight="1">
       <c r="A37" s="13" t="inlineStr">
         <is>
-          <t>EGR801554045</t>
+          <t>EGR996764210</t>
         </is>
       </c>
       <c r="B37" s="5" t="inlineStr">
         <is>
-          <t>BGR159031301000, TGR801554045, L213800YJOZGHVAPEJP93</t>
+          <t>TGR996764210, BGR157802360000</t>
         </is>
       </c>
       <c r="C37" s="14" t="n">
-        <v>44302</v>
+        <v>44210</v>
       </c>
       <c r="D37" s="5" t="inlineStr">
         <is>
-          <t>SIREC ENERGY CAPITAL PARTNERS ΜΟΝΟΠΡΟΣΩΠΗ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>ΣΥΜΜΕΤΟΧΕΣ 5G Ανώνυμη Εταιρεία</t>
         </is>
       </c>
       <c r="E37" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01059</t>
+          <t>EGRAK01067</t>
         </is>
       </c>
       <c r="F37" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01059</t>
+          <t>EGRAK01067</t>
         </is>
       </c>
     </row>
     <row r="38" ht="36" customHeight="1">
       <c r="A38" s="11" t="inlineStr">
         <is>
-          <t>EGRAEEAP009</t>
+          <t>EGR801554045</t>
         </is>
       </c>
       <c r="B38" s="7" t="inlineStr">
         <is>
-          <t>BGR160110060000, L2138006STLTDFRIZTC42, TGR996805731</t>
+          <t>L213800YJOZGHVAPEJP93, TGR801554045, BGR159031301000</t>
         </is>
       </c>
       <c r="C38" s="12" t="n">
-        <v>44389</v>
+        <v>44302</v>
       </c>
       <c r="D38" s="7" t="inlineStr">
         <is>
-          <t>TRADE ESTATES ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΑΚΙΝΗΤΗΣ ΠΕΡΙΟΥΣΙΑΣ</t>
-        </is>
-      </c>
-      <c r="E38" s="7" t="inlineStr"/>
+          <t>SIREC ENERGY CAPITAL PARTNERS ΜΟΝΟΠΡΟΣΩΠΗ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+        </is>
+      </c>
+      <c r="E38" s="7" t="inlineStr">
+        <is>
+          <t>EGRAK01059</t>
+        </is>
+      </c>
       <c r="F38" s="7" t="inlineStr">
         <is>
-          <t>EGRAEEAP009</t>
+          <t>EGRAK01059</t>
         </is>
       </c>
     </row>
     <row r="39" ht="36" customHeight="1">
       <c r="A39" s="13" t="inlineStr">
         <is>
-          <t>EGR801698110</t>
+          <t>EGRAEEAP009</t>
         </is>
       </c>
       <c r="B39" s="5" t="inlineStr">
         <is>
-          <t>BGR161709401000, L984500E6O0A11A6C4E59, TGR801698110</t>
+          <t>L2138006STLTDFRIZTC42, TGR996805731, BGR160110060000</t>
         </is>
       </c>
       <c r="C39" s="14" t="n">
-        <v>44524</v>
+        <v>44389</v>
       </c>
       <c r="D39" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">ELBRIDGE CAPITAL MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΗΣΗΣ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΙΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ </t>
-        </is>
-      </c>
-      <c r="E39" s="5" t="inlineStr">
-        <is>
-          <t>EGRAK01103</t>
-        </is>
-      </c>
+          <t>TRADE ESTATES ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΑΚΙΝΗΤΗΣ ΠΕΡΙΟΥΣΙΑΣ</t>
+        </is>
+      </c>
+      <c r="E39" s="5" t="inlineStr"/>
       <c r="F39" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01103</t>
+          <t>EGRAEEAP009</t>
         </is>
       </c>
     </row>
     <row r="40" ht="36" customHeight="1">
       <c r="A40" s="11" t="inlineStr">
         <is>
-          <t>EGR094321237</t>
+          <t>EGR801698110</t>
         </is>
       </c>
       <c r="B40" s="7" t="inlineStr">
         <is>
-          <t>L213800MU91F1752AVM79, BGR000861301000, TGR094321237</t>
+          <t>BGR161709401000, L984500E6O0A11A6C4E59, TGR801698110</t>
         </is>
       </c>
       <c r="C40" s="12" t="n">
-        <v>44635</v>
+        <v>44524</v>
       </c>
       <c r="D40" s="7" t="inlineStr">
         <is>
-          <t>PREMIA ΑΝΩΝΥΜΟΣ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΣΕ ΑΚΙΝΗΤΗ ΠΕΡΙΟΥΣΙΑ</t>
-        </is>
-      </c>
-      <c r="E40" s="7" t="inlineStr"/>
+          <t xml:space="preserve">ELBRIDGE CAPITAL MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΗΣΗΣ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΙΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ </t>
+        </is>
+      </c>
+      <c r="E40" s="7" t="inlineStr">
+        <is>
+          <t>EGRAK01103</t>
+        </is>
+      </c>
       <c r="F40" s="7" t="inlineStr">
         <is>
-          <t>EGR094321237</t>
+          <t>EGRAK01103</t>
         </is>
       </c>
     </row>
     <row r="41" ht="36" customHeight="1">
       <c r="A41" s="13" t="inlineStr">
         <is>
-          <t>EGR801812106</t>
+          <t>EGR094321237</t>
         </is>
       </c>
       <c r="B41" s="5" t="inlineStr">
         <is>
-          <t>TGR801812106, BGR163809001000</t>
+          <t>TGR094321237, BGR000861301000, L213800MU91F1752AVM79</t>
         </is>
       </c>
       <c r="C41" s="14" t="n">
-        <v>44665</v>
+        <v>44635</v>
       </c>
       <c r="D41" s="5" t="inlineStr">
         <is>
-          <t>LSTONE ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
-        </is>
-      </c>
-      <c r="E41" s="5" t="inlineStr">
-        <is>
-          <t>EGRAK01072</t>
-        </is>
-      </c>
+          <t>PREMIA ΑΝΩΝΥΜΟΣ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΣΕ ΑΚΙΝΗΤΗ ΠΕΡΙΟΥΣΙΑ</t>
+        </is>
+      </c>
+      <c r="E41" s="5" t="inlineStr"/>
       <c r="F41" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01072</t>
+          <t>EGR094321237</t>
         </is>
       </c>
     </row>
     <row r="42" ht="36" customHeight="1">
       <c r="A42" s="11" t="inlineStr">
         <is>
-          <t>EGR801878297</t>
+          <t>EGR801812106</t>
         </is>
       </c>
       <c r="B42" s="7" t="inlineStr">
         <is>
-          <t>L984500F87AF5652C5A91, BGR165052501000, TGR801878297</t>
+          <t>TGR801812106, BGR163809001000</t>
         </is>
       </c>
       <c r="C42" s="12" t="n">
-        <v>44760</v>
+        <v>44665</v>
       </c>
       <c r="D42" s="7" t="inlineStr">
         <is>
-          <t>BIG PI ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>LSTONE ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E42" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01073</t>
+          <t>EGRAK01072</t>
         </is>
       </c>
       <c r="F42" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01073</t>
+          <t>EGRAK01072</t>
         </is>
       </c>
     </row>
     <row r="43" ht="36" customHeight="1">
       <c r="A43" s="13" t="inlineStr">
         <is>
-          <t>EGR802025852</t>
+          <t>EGR801878297</t>
         </is>
       </c>
       <c r="B43" s="5" t="inlineStr">
         <is>
-          <t>BGR168398401000, TGR802025852</t>
+          <t>L984500F87AF5652C5A91, TGR801878297, BGR165052501000</t>
         </is>
       </c>
       <c r="C43" s="14" t="n">
-        <v>44953</v>
+        <v>44760</v>
       </c>
       <c r="D43" s="5" t="inlineStr">
         <is>
-          <t>IGROW VENTURE PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ Α.Ε.</t>
+          <t>BIG PI ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E43" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01100</t>
+          <t>EGRAK01073</t>
         </is>
       </c>
       <c r="F43" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01100</t>
+          <t>EGRAK01073</t>
         </is>
       </c>
     </row>
     <row r="44" ht="36" customHeight="1">
       <c r="A44" s="11" t="inlineStr">
         <is>
-          <t>EGR802047322</t>
+          <t>EGR802025852</t>
         </is>
       </c>
       <c r="B44" s="7" t="inlineStr">
         <is>
-          <t>TGR802047322, BGR168862301000, L2138007QOK3W75DIHX50</t>
+          <t>BGR168398401000, TGR802025852</t>
         </is>
       </c>
       <c r="C44" s="12" t="n">
-        <v>44972</v>
+        <v>44953</v>
       </c>
       <c r="D44" s="7" t="inlineStr">
         <is>
-          <t>SPOROS Impact Ventures ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ Διαχείρισης Αμοιβαίων Κεφαλαίων Επιχειρηματικών Συμμετοχών</t>
+          <t>IGROW VENTURE PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ Α.Ε.</t>
         </is>
       </c>
       <c r="E44" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01075</t>
+          <t>EGRAK01100</t>
         </is>
       </c>
       <c r="F44" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01075</t>
+          <t>EGRAK01100</t>
         </is>
       </c>
     </row>
     <row r="45" ht="36" customHeight="1">
       <c r="A45" s="13" t="inlineStr">
         <is>
-          <t>EGR802071555</t>
+          <t>EGR802047322</t>
         </is>
       </c>
       <c r="B45" s="5" t="inlineStr">
         <is>
-          <t>BGR169369101000, TGR802071555</t>
+          <t>TGR802047322, BGR168862301000, L2138007QOK3W75DIHX50</t>
         </is>
       </c>
       <c r="C45" s="14" t="n">
-        <v>44995</v>
+        <v>44972</v>
       </c>
       <c r="D45" s="5" t="inlineStr">
         <is>
-          <t>FOS CAPITAL MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>SPOROS Impact Ventures ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ Διαχείρισης Αμοιβαίων Κεφαλαίων Επιχειρηματικών Συμμετοχών</t>
         </is>
       </c>
       <c r="E45" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01076</t>
+          <t>EGRAK01075</t>
         </is>
       </c>
       <c r="F45" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01076</t>
+          <t>EGRAK01075</t>
         </is>
       </c>
     </row>
     <row r="46" ht="36" customHeight="1">
       <c r="A46" s="11" t="inlineStr">
         <is>
-          <t>EGR802177269</t>
+          <t>EGR802071555</t>
         </is>
       </c>
       <c r="B46" s="7" t="inlineStr">
         <is>
-          <t>TGR802177269, BGR171519601000, L984500EE58FDEBF8BF32</t>
+          <t>BGR169369101000, TGR802071555</t>
         </is>
       </c>
       <c r="C46" s="12" t="n">
-        <v>45114</v>
+        <v>44995</v>
       </c>
       <c r="D46" s="7" t="inlineStr">
         <is>
-          <t>OIKOS FUND MANAGEMENT ΑΜΟΙΒΑΙΑ ΚΕΦΑΛΑΙΑ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ</t>
+          <t>FOS CAPITAL MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E46" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01074</t>
+          <t>EGRAK01076</t>
         </is>
       </c>
       <c r="F46" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01074</t>
+          <t>EGRAK01076</t>
         </is>
       </c>
     </row>
     <row r="47" ht="36" customHeight="1">
       <c r="A47" s="13" t="inlineStr">
         <is>
-          <t>EGR802187644</t>
+          <t>EGR802177269</t>
         </is>
       </c>
       <c r="B47" s="5" t="inlineStr">
         <is>
-          <t>TGR802187644, BGR171720006000</t>
+          <t>TGR802177269, BGR171519601000, L984500EE58FDEBF8BF32</t>
         </is>
       </c>
       <c r="C47" s="14" t="n">
-        <v>45128</v>
+        <v>45114</v>
       </c>
       <c r="D47" s="5" t="inlineStr">
         <is>
-          <t>LOGGERHEAD VENTURES ΑΜΟΙΒΑΙΑ ΚΕΦΑΛΑΙΑ ΕΠΙΧΕΙΡΙΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ</t>
+          <t>OIKOS FUND MANAGEMENT ΑΜΟΙΒΑΙΑ ΚΕΦΑΛΑΙΑ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ</t>
         </is>
       </c>
       <c r="E47" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01104</t>
+          <t>EGRAK01074</t>
         </is>
       </c>
       <c r="F47" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01104</t>
+          <t>EGRAK01074</t>
         </is>
       </c>
     </row>
     <row r="48" ht="36" customHeight="1">
       <c r="A48" s="11" t="inlineStr">
         <is>
-          <t>EGR802190685</t>
+          <t>EGR802187644</t>
         </is>
       </c>
       <c r="B48" s="7" t="inlineStr">
         <is>
-          <t>BGR171775701000, TGR802190685</t>
+          <t>BGR171720006000, TGR802187644</t>
         </is>
       </c>
       <c r="C48" s="12" t="n">
-        <v>45134</v>
+        <v>45128</v>
       </c>
       <c r="D48" s="7" t="inlineStr">
         <is>
-          <t>APEIRON VENTURES CAPITAL PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
+          <t>LOGGERHEAD VENTURES ΑΜΟΙΒΑΙΑ ΚΕΦΑΛΑΙΑ ΕΠΙΧΕΙΡΙΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ</t>
         </is>
       </c>
       <c r="E48" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01099</t>
+          <t>EGRAK01104</t>
         </is>
       </c>
       <c r="F48" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01099</t>
+          <t>EGRAK01104</t>
         </is>
       </c>
     </row>
     <row r="49" ht="36" customHeight="1">
       <c r="A49" s="13" t="inlineStr">
         <is>
-          <t>EGR802300393</t>
+          <t>EGR802190685</t>
         </is>
       </c>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>TGR802300393, BGR173916401000</t>
+          <t>BGR171775701000, TGR802190685</t>
         </is>
       </c>
       <c r="C49" s="14" t="n">
-        <v>45273</v>
+        <v>45134</v>
       </c>
       <c r="D49" s="5" t="inlineStr">
         <is>
-          <t>GOLDEN AGE CAPITAL A.E.D.A.K.E.S.</t>
+          <t>APEIRON VENTURES CAPITAL PARTNERS ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E49" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01129</t>
+          <t>EGRAK01099</t>
         </is>
       </c>
       <c r="F49" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01129</t>
+          <t>EGRAK01099</t>
         </is>
       </c>
     </row>
     <row r="50" ht="36" customHeight="1">
       <c r="A50" s="11" t="inlineStr">
         <is>
-          <t>EGRMFMC023</t>
+          <t>EGR802300393</t>
         </is>
       </c>
       <c r="B50" s="7" t="inlineStr">
         <is>
-          <t>TGR996542649, BGR173975960000, L213800G7J7NDXVAS3P11</t>
+          <t>BGR173916401000, TGR802300393</t>
         </is>
       </c>
       <c r="C50" s="12" t="n">
-        <v>45278</v>
+        <v>45273</v>
       </c>
       <c r="D50" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TRUST Μονοπρόσωπη Ανώνυμη Εταιρεία Διαχείρισης Αμοιβαίων Κεφαλαίων και Οργανισμών Εναλλακτικών Επενδύσεων</t>
+          <t>GOLDEN AGE CAPITAL A.E.D.A.K.E.S.</t>
         </is>
       </c>
       <c r="E50" s="7" t="inlineStr">
         <is>
-          <t>EGRAK00020, EGRAK00106, EGRAK00135, EGRAK00205, EGRAK00206, EGRAK00443, EGRAK00462, EGRAK00820, EGRAK00827, EGRAK00850, EGRAK00892, EGRAK01001, EGRAK01110</t>
+          <t>EGRAK01129</t>
         </is>
       </c>
       <c r="F50" s="7" t="inlineStr">
         <is>
-          <t>EGRAK00020, EGRAK00106, EGRAK00135, EGRAK00205, EGRAK00206, EGRAK00443, EGRAK00462, EGRAK00820, EGRAK00827, EGRAK00850, EGRAK00892, EGRAK01001, EGRAK01110</t>
+          <t>EGRAK01129</t>
         </is>
       </c>
     </row>
     <row r="51" ht="36" customHeight="1">
       <c r="A51" s="13" t="inlineStr">
         <is>
-          <t>EGRAEEAP012</t>
+          <t>EGRMFMC023</t>
         </is>
       </c>
       <c r="B51" s="5" t="inlineStr">
         <is>
-          <t>TGR996723817, BGR174106158000</t>
+          <t>L213800G7J7NDXVAS3P11, TGR996542649, BGR173975960000</t>
         </is>
       </c>
       <c r="C51" s="14" t="n">
-        <v>45287</v>
+        <v>45278</v>
       </c>
       <c r="D51" s="5" t="inlineStr">
         <is>
-          <t>ΜΟΝΟΠΡΟΣΩΠΗ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΑΚΙΝΗΤΗΣ ΠΕΡΙΟΥΣΙΑΣ ΧΑΝΙΩΝ</t>
-        </is>
-      </c>
-      <c r="E51" s="5" t="inlineStr"/>
+          <t>ALPHA TRUST Μονοπρόσωπη Ανώνυμη Εταιρεία Διαχείρισης Αμοιβαίων Κεφαλαίων και Οργανισμών Εναλλακτικών Επενδύσεων</t>
+        </is>
+      </c>
+      <c r="E51" s="5" t="inlineStr">
+        <is>
+          <t>EGRAK00020, EGRAK00106, EGRAK00135, EGRAK00205, EGRAK00206, EGRAK00443, EGRAK00462, EGRAK00820, EGRAK00827, EGRAK00850, EGRAK00892, EGRAK01001, EGRAK01110</t>
+        </is>
+      </c>
       <c r="F51" s="5" t="inlineStr">
         <is>
-          <t>EGRAEEAP012</t>
+          <t>EGRAK00020, EGRAK00106, EGRAK00135, EGRAK00205, EGRAK00206, EGRAK00443, EGRAK00462, EGRAK00820, EGRAK00827, EGRAK00850, EGRAK00892, EGRAK01001, EGRAK01110</t>
         </is>
       </c>
     </row>
     <row r="52" ht="36" customHeight="1">
       <c r="A52" s="11" t="inlineStr">
         <is>
-          <t>EGR802458356</t>
+          <t>EGRAEEAP012</t>
         </is>
       </c>
       <c r="B52" s="7" t="inlineStr">
         <is>
-          <t>TGR802458356, BGR176733801000</t>
+          <t>BGR174106158000, TGR996723817</t>
         </is>
       </c>
       <c r="C52" s="12" t="n">
-        <v>45392</v>
+        <v>45287</v>
       </c>
       <c r="D52" s="7" t="inlineStr">
         <is>
-          <t>CORALLIA VENTURES MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
-        </is>
-      </c>
-      <c r="E52" s="7" t="inlineStr">
-        <is>
-          <t>EGRAK01102</t>
-        </is>
-      </c>
+          <t>ΜΟΝΟΠΡΟΣΩΠΗ ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΕΠΕΝΔΥΣΕΩΝ ΑΚΙΝΗΤΗΣ ΠΕΡΙΟΥΣΙΑΣ ΧΑΝΙΩΝ</t>
+        </is>
+      </c>
+      <c r="E52" s="7" t="inlineStr"/>
       <c r="F52" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01102</t>
+          <t>EGRAEEAP012</t>
         </is>
       </c>
     </row>
     <row r="53" ht="36" customHeight="1">
       <c r="A53" s="13" t="inlineStr">
         <is>
-          <t>EGR802504273</t>
+          <t>EGR802458356</t>
         </is>
       </c>
       <c r="B53" s="5" t="inlineStr">
         <is>
-          <t>TGR802504273, BGR177617001000</t>
+          <t>TGR802458356, BGR176733801000</t>
         </is>
       </c>
       <c r="C53" s="14" t="n">
-        <v>45440</v>
+        <v>45392</v>
       </c>
       <c r="D53" s="5" t="inlineStr">
         <is>
-          <t>SUSTAINABLE FORWARD CAPITAL Α.Ε.Δ.Α.Κ.Ε.Σ.</t>
+          <t>CORALLIA VENTURES MANAGEMENT ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
       <c r="E53" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01127</t>
+          <t>EGRAK01102</t>
         </is>
       </c>
       <c r="F53" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01127</t>
+          <t>EGRAK01102</t>
         </is>
       </c>
     </row>
     <row r="54" ht="36" customHeight="1">
       <c r="A54" s="11" t="inlineStr">
         <is>
+          <t>EGR802504273</t>
+        </is>
+      </c>
+      <c r="B54" s="7" t="inlineStr">
+        <is>
+          <t>BGR177617001000, TGR802504273</t>
+        </is>
+      </c>
+      <c r="C54" s="12" t="n">
+        <v>45440</v>
+      </c>
+      <c r="D54" s="7" t="inlineStr">
+        <is>
+          <t>SUSTAINABLE FORWARD CAPITAL Α.Ε.Δ.Α.Κ.Ε.Σ.</t>
+        </is>
+      </c>
+      <c r="E54" s="7" t="inlineStr">
+        <is>
+          <t>EGRAK01127</t>
+        </is>
+      </c>
+      <c r="F54" s="7" t="inlineStr">
+        <is>
+          <t>EGRAK01127</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" ht="36" customHeight="1">
+      <c r="A55" s="13" t="inlineStr">
+        <is>
           <t>EGR802560246</t>
         </is>
       </c>
-      <c r="B54" s="7" t="inlineStr">
+      <c r="B55" s="5" t="inlineStr">
         <is>
           <t>BGR178614401000, TGR802560246</t>
         </is>
       </c>
-      <c r="C54" s="12" t="n">
+      <c r="C55" s="14" t="n">
         <v>45502</v>
       </c>
-      <c r="D54" s="7" t="inlineStr">
+      <c r="D55" s="5" t="inlineStr">
         <is>
           <t>EVERCURIOUS VC ΑΝΩΝΥΜΗ ΕΤΑΙΡΕΙΑ ΔΙΑΧΕΙΡΙΣΗΣ ΑΜΟΙΒΑΙΩΝ ΚΕΦΑΛΑΙΩΝ ΕΠΙΧΕΙΡΗΜΑΤΙΚΩΝ ΣΥΜΜΕΤΟΧΩΝ</t>
         </is>
       </c>
-      <c r="E54" s="7" t="inlineStr">
+      <c r="E55" s="5" t="inlineStr">
         <is>
           <t>EGRAK01128</t>
         </is>
       </c>
-      <c r="F54" s="7" t="inlineStr">
+      <c r="F55" s="5" t="inlineStr">
         <is>
           <t>EGRAK01128</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F54"/>
+  <autoFilter ref="A1:F55"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2691,7 +2721,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J271"/>
+  <dimension ref="A1:J270"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -5163,7 +5193,7 @@
       </c>
       <c r="B59" s="5" t="inlineStr">
         <is>
-          <t>TGR099759863, BGR003882701000, L213800USGL7Q5UR9M221</t>
+          <t>BGR003882701000, L213800USGL7Q5UR9M221, TGR099759863</t>
         </is>
       </c>
       <c r="C59" s="14" t="n">
@@ -8133,7 +8163,7 @@
       </c>
       <c r="B130" s="7" t="inlineStr">
         <is>
-          <t>TGR997656128, L213800Q23BDHSW1OQT90, BGR128686346000</t>
+          <t>TGR997656128, BGR128686346000, L213800Q23BDHSW1OQT90</t>
         </is>
       </c>
       <c r="C130" s="12" t="n">
@@ -8213,7 +8243,7 @@
       </c>
       <c r="B132" s="7" t="inlineStr">
         <is>
-          <t>L213800DDNBUCO6A2RT84, BGR131359701000, TGR800596087</t>
+          <t>TGR800596087, L213800DDNBUCO6A2RT84, BGR131359701000</t>
         </is>
       </c>
       <c r="C132" s="12" t="n">
@@ -8847,7 +8877,7 @@
       </c>
       <c r="B147" s="5" t="inlineStr">
         <is>
-          <t>L213800DTEZE6R8BZ9K19, BGR148547901000, TGR801077433</t>
+          <t>BGR148547901000, L213800DTEZE6R8BZ9K19, TGR801077433</t>
         </is>
       </c>
       <c r="C147" s="14" t="n">
@@ -9015,7 +9045,7 @@
       </c>
       <c r="B151" s="5" t="inlineStr">
         <is>
-          <t>TGR996899546, L213800XKY8GHKN57D970, BGR152321260000</t>
+          <t>L213800XKY8GHKN57D970, BGR152321260000, TGR996899546</t>
         </is>
       </c>
       <c r="C151" s="14" t="n">
@@ -9615,7 +9645,7 @@
       </c>
       <c r="B165" s="5" t="inlineStr">
         <is>
-          <t>BGR160110060000, L2138006STLTDFRIZTC42, TGR996805731</t>
+          <t>L2138006STLTDFRIZTC42, TGR996805731, BGR160110060000</t>
         </is>
       </c>
       <c r="C165" s="14" t="n">
@@ -9863,7 +9893,7 @@
       </c>
       <c r="B171" s="5" t="inlineStr">
         <is>
-          <t>L213800MU91F1752AVM79, BGR000861301000, TGR094321237</t>
+          <t>TGR094321237, BGR000861301000, L213800MU91F1752AVM79</t>
         </is>
       </c>
       <c r="C171" s="14" t="n">
@@ -10096,15 +10126,19 @@
       </c>
       <c r="G176" s="7" t="inlineStr">
         <is>
-          <t>EGR800398384</t>
+          <t>EGR099757323</t>
         </is>
       </c>
       <c r="H176" s="7" t="inlineStr">
         <is>
-          <t>EGR800398384</t>
-        </is>
-      </c>
-      <c r="I176" s="7" t="inlineStr"/>
+          <t>EGR099757323</t>
+        </is>
+      </c>
+      <c r="I176" s="7" t="inlineStr">
+        <is>
+          <t>IGRF000506003</t>
+        </is>
+      </c>
       <c r="J176" s="7" t="inlineStr"/>
     </row>
     <row r="177" ht="36" customHeight="1">
@@ -10745,7 +10779,7 @@
       </c>
       <c r="B192" s="7" t="inlineStr">
         <is>
-          <t>L213800986AE336VYQP62,  L213800986AE336VYQP62</t>
+          <t>L213800986AE336VYQP62</t>
         </is>
       </c>
       <c r="C192" s="12" t="n">
@@ -12081,7 +12115,7 @@
       </c>
       <c r="B224" s="7" t="inlineStr">
         <is>
-          <t>TGR996723817, BGR174106158000</t>
+          <t>BGR174106158000, TGR996723817</t>
         </is>
       </c>
       <c r="C224" s="12" t="n">
@@ -12245,7 +12279,7 @@
       </c>
       <c r="B228" s="7" t="inlineStr">
         <is>
-          <t>L213800JLK8K87ENMO7297</t>
+          <t>L213800JLK8K87ENMO729</t>
         </is>
       </c>
       <c r="C228" s="12" t="n">
@@ -14043,50 +14077,8 @@
       </c>
       <c r="J270" s="7" t="inlineStr"/>
     </row>
-    <row r="271" ht="36" customHeight="1">
-      <c r="A271" s="13" t="inlineStr">
-        <is>
-          <t>EGRAK01122</t>
-        </is>
-      </c>
-      <c r="B271" s="5" t="inlineStr">
-        <is>
-          <t>L21380014H6B458ZBEZ73</t>
-        </is>
-      </c>
-      <c r="C271" s="14" t="n">
-        <v>45747</v>
-      </c>
-      <c r="D271" s="5" t="inlineStr">
-        <is>
-          <t>ΠΕΙΡΑΙΩΣ Α/Κ ΕΙΣΟΔΗΜΑΤΟΣ 2025 ΕΥΡΩΠΑΪΚΟ ΟΜΟΛΟΓΙΑΚΟ</t>
-        </is>
-      </c>
-      <c r="E271" s="5" t="inlineStr">
-        <is>
-          <t>BON</t>
-        </is>
-      </c>
-      <c r="F271" s="5" t="inlineStr"/>
-      <c r="G271" s="5" t="inlineStr">
-        <is>
-          <t>EGRMFMC015</t>
-        </is>
-      </c>
-      <c r="H271" s="5" t="inlineStr">
-        <is>
-          <t>EGRMFMC015</t>
-        </is>
-      </c>
-      <c r="I271" s="5" t="inlineStr">
-        <is>
-          <t>IGRF000460003</t>
-        </is>
-      </c>
-      <c r="J271" s="5" t="inlineStr"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J271"/>
+  <autoFilter ref="A1:J270"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -14097,7 +14089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D362"/>
+  <dimension ref="A1:D363"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -14111,7 +14103,7 @@
     <col width="23.4" customWidth="1" min="1" max="1"/>
     <col width="27.3" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="31.2" customWidth="1" min="4" max="4"/>
+    <col width="18.2" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="42" customHeight="1">
@@ -19174,63 +19166,59 @@
     <row r="258" ht="36" customHeight="1">
       <c r="A258" s="11" t="inlineStr">
         <is>
-          <t>IGRF000392008</t>
+          <t>IGRF000506003</t>
         </is>
       </c>
       <c r="B258" s="12" t="n">
-        <v>44846</v>
-      </c>
-      <c r="C258" s="7" t="inlineStr">
-        <is>
-          <t>Alpha Bancassurance EE104 Structured Fund</t>
-        </is>
-      </c>
+        <v>44827</v>
+      </c>
+      <c r="C258" s="7" t="inlineStr"/>
       <c r="D258" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01015</t>
+          <t>EGRAK01057</t>
         </is>
       </c>
     </row>
     <row r="259" ht="36" customHeight="1">
       <c r="A259" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01072_SHR</t>
+          <t>IGRF000392008</t>
         </is>
       </c>
       <c r="B259" s="14" t="n">
-        <v>44851</v>
-      </c>
-      <c r="C259" s="5" t="inlineStr"/>
+        <v>44846</v>
+      </c>
+      <c r="C259" s="5" t="inlineStr">
+        <is>
+          <t>Alpha Bancassurance EE104 Structured Fund</t>
+        </is>
+      </c>
       <c r="D259" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01072</t>
+          <t>EGRAK01015</t>
         </is>
       </c>
     </row>
     <row r="260" ht="36" customHeight="1">
       <c r="A260" s="11" t="inlineStr">
         <is>
-          <t>IGRF000393006</t>
+          <t>PEGRAK01072_SHR</t>
         </is>
       </c>
       <c r="B260" s="12" t="n">
-        <v>44865</v>
-      </c>
-      <c r="C260" s="7" t="inlineStr">
-        <is>
-          <t>Alpha Prosperity I 90-140 Structured Fund</t>
-        </is>
-      </c>
+        <v>44851</v>
+      </c>
+      <c r="C260" s="7" t="inlineStr"/>
       <c r="D260" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01016</t>
+          <t>EGRAK01072</t>
         </is>
       </c>
     </row>
     <row r="261" ht="36" customHeight="1">
       <c r="A261" s="13" t="inlineStr">
         <is>
-          <t>IGRF000394004</t>
+          <t>IGRF000393006</t>
         </is>
       </c>
       <c r="B261" s="14" t="n">
@@ -19238,235 +19226,235 @@
       </c>
       <c r="C261" s="5" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME 5year - BOND FUND</t>
+          <t>Alpha Prosperity I 90-140 Structured Fund</t>
         </is>
       </c>
       <c r="D261" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01013</t>
+          <t>EGRAK01016</t>
         </is>
       </c>
     </row>
     <row r="262" ht="36" customHeight="1">
       <c r="A262" s="11" t="inlineStr">
         <is>
-          <t>IGRF000395001</t>
+          <t>IGRF000394004</t>
         </is>
       </c>
       <c r="B262" s="12" t="n">
-        <v>44873</v>
+        <v>44865</v>
       </c>
       <c r="C262" s="7" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2027 DOMESTIC BOND FUND</t>
+          <t>DELOS EXTRA INCOME 5year - BOND FUND</t>
         </is>
       </c>
       <c r="D262" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01014</t>
+          <t>EGRAK01013</t>
         </is>
       </c>
     </row>
     <row r="263" ht="36" customHeight="1">
       <c r="A263" s="13" t="inlineStr">
         <is>
-          <t>IGRF000397007</t>
+          <t>IGRF000395001</t>
         </is>
       </c>
       <c r="B263" s="14" t="n">
-        <v>44879</v>
+        <v>44873</v>
       </c>
       <c r="C263" s="5" t="inlineStr">
         <is>
-          <t>EUROBANK DIS GF Target Maturity II Bond Fund</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2027 DOMESTIC BOND FUND</t>
         </is>
       </c>
       <c r="D263" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01017</t>
+          <t>EGRAK01014</t>
         </is>
       </c>
     </row>
     <row r="264" ht="36" customHeight="1">
       <c r="A264" s="11" t="inlineStr">
         <is>
-          <t>IGRF000408002</t>
+          <t>IGRF000397007</t>
         </is>
       </c>
       <c r="B264" s="12" t="n">
-        <v>44936</v>
+        <v>44879</v>
       </c>
       <c r="C264" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TARGET MATURITY I 2028 BOND FUND Classic D</t>
+          <t>EUROBANK DIS GF Target Maturity II Bond Fund</t>
         </is>
       </c>
       <c r="D264" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01019</t>
+          <t>EGRAK01017</t>
         </is>
       </c>
     </row>
     <row r="265" ht="36" customHeight="1">
       <c r="A265" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01073_SHR</t>
+          <t>IGRF000408002</t>
         </is>
       </c>
       <c r="B265" s="14" t="n">
-        <v>44944</v>
-      </c>
-      <c r="C265" s="5" t="inlineStr"/>
+        <v>44936</v>
+      </c>
+      <c r="C265" s="5" t="inlineStr">
+        <is>
+          <t>ALPHA TARGET MATURITY I 2028 BOND FUND Classic D</t>
+        </is>
+      </c>
       <c r="D265" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01073</t>
+          <t>EGRAK01019</t>
         </is>
       </c>
     </row>
     <row r="266" ht="36" customHeight="1">
       <c r="A266" s="11" t="inlineStr">
         <is>
-          <t>IGRF000411006</t>
+          <t>PEGRAK01073_SHR</t>
         </is>
       </c>
       <c r="B266" s="12" t="n">
-        <v>44951</v>
-      </c>
-      <c r="C266" s="7" t="inlineStr">
-        <is>
-          <t>EUROBANK DIS GF TARGET MATURITY III BOND FUND</t>
-        </is>
-      </c>
+        <v>44944</v>
+      </c>
+      <c r="C266" s="7" t="inlineStr"/>
       <c r="D266" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01021</t>
+          <t>EGRAK01073</t>
         </is>
       </c>
     </row>
     <row r="267" ht="36" customHeight="1">
       <c r="A267" s="13" t="inlineStr">
         <is>
-          <t>IGRF000409000</t>
+          <t>IGRF000411006</t>
         </is>
       </c>
       <c r="B267" s="14" t="n">
-        <v>44963</v>
+        <v>44951</v>
       </c>
       <c r="C267" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2028 EUROPEAN BOND FUND</t>
+          <t>EUROBANK DIS GF TARGET MATURITY III BOND FUND</t>
         </is>
       </c>
       <c r="D267" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01018</t>
+          <t>EGRAK01021</t>
         </is>
       </c>
     </row>
     <row r="268" ht="36" customHeight="1">
       <c r="A268" s="11" t="inlineStr">
         <is>
-          <t>IGRF000417003</t>
+          <t>IGRF000409000</t>
         </is>
       </c>
       <c r="B268" s="12" t="n">
-        <v>44971</v>
+        <v>44963</v>
       </c>
       <c r="C268" s="7" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME II 5year - BOND FUND</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2028 EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D268" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01020</t>
+          <t>EGRAK01018</t>
         </is>
       </c>
     </row>
     <row r="269" ht="36" customHeight="1">
       <c r="A269" s="13" t="inlineStr">
         <is>
-          <t>IGRF000412004</t>
+          <t>IGRF000417003</t>
         </is>
       </c>
       <c r="B269" s="14" t="n">
-        <v>44972</v>
+        <v>44971</v>
       </c>
       <c r="C269" s="5" t="inlineStr">
         <is>
-          <t>EUROBANK  GF TARGET MATURITY IV BOND FUND</t>
+          <t>DELOS EXTRA INCOME II 5year - BOND FUND</t>
         </is>
       </c>
       <c r="D269" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01023</t>
+          <t>EGRAK01020</t>
         </is>
       </c>
     </row>
     <row r="270" ht="36" customHeight="1">
       <c r="A270" s="11" t="inlineStr">
         <is>
-          <t>IGRF000418001</t>
+          <t>IGRF000412004</t>
         </is>
       </c>
       <c r="B270" s="12" t="n">
-        <v>44977</v>
+        <v>44972</v>
       </c>
       <c r="C270" s="7" t="inlineStr">
         <is>
-          <t>Optima greek income bond fund</t>
+          <t>EUROBANK  GF TARGET MATURITY IV BOND FUND</t>
         </is>
       </c>
       <c r="D270" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01022</t>
+          <t>EGRAK01023</t>
         </is>
       </c>
     </row>
     <row r="271" ht="36" customHeight="1">
       <c r="A271" s="13" t="inlineStr">
         <is>
-          <t>IGRF000423001</t>
+          <t>IGRF000418001</t>
         </is>
       </c>
       <c r="B271" s="14" t="n">
-        <v>45005</v>
+        <v>44977</v>
       </c>
       <c r="C271" s="5" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME III 5year - BOND FUND</t>
+          <t>Optima greek income bond fund</t>
         </is>
       </c>
       <c r="D271" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01026</t>
+          <t>EGRAK01022</t>
         </is>
       </c>
     </row>
     <row r="272" ht="36" customHeight="1">
       <c r="A272" s="11" t="inlineStr">
         <is>
-          <t>IGRF000421005</t>
+          <t>IGRF000423001</t>
         </is>
       </c>
       <c r="B272" s="12" t="n">
-        <v>45019</v>
+        <v>45005</v>
       </c>
       <c r="C272" s="7" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2028 II EUROPEAN BOND FUND</t>
+          <t>DELOS EXTRA INCOME III 5year - BOND FUND</t>
         </is>
       </c>
       <c r="D272" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01048</t>
+          <t>EGRAK01026</t>
         </is>
       </c>
     </row>
     <row r="273" ht="36" customHeight="1">
       <c r="A273" s="13" t="inlineStr">
         <is>
-          <t>IGRF000422003</t>
+          <t>IGRF000421005</t>
         </is>
       </c>
       <c r="B273" s="14" t="n">
@@ -19474,39 +19462,39 @@
       </c>
       <c r="C273" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2029 EUROPEAN BOND FUND</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2028 II EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D273" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01028</t>
+          <t>EGRAK01048</t>
         </is>
       </c>
     </row>
     <row r="274" ht="36" customHeight="1">
       <c r="A274" s="11" t="inlineStr">
         <is>
-          <t>IGRF000426004</t>
+          <t>IGRF000422003</t>
         </is>
       </c>
       <c r="B274" s="12" t="n">
-        <v>45021</v>
+        <v>45019</v>
       </c>
       <c r="C274" s="7" t="inlineStr">
         <is>
-          <t>TRITON Maximizer Conservative Fund of Funds Class A</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2029 EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D274" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01031</t>
+          <t>EGRAK01028</t>
         </is>
       </c>
     </row>
     <row r="275" ht="36" customHeight="1">
       <c r="A275" s="13" t="inlineStr">
         <is>
-          <t>IGRF000428000</t>
+          <t>IGRF000426004</t>
         </is>
       </c>
       <c r="B275" s="14" t="n">
@@ -19514,19 +19502,19 @@
       </c>
       <c r="C275" s="5" t="inlineStr">
         <is>
-          <t>TRITON Maximizer Balanced Fund of Funds Class A</t>
+          <t>TRITON Maximizer Conservative Fund of Funds Class A</t>
         </is>
       </c>
       <c r="D275" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01030</t>
+          <t>EGRAK01031</t>
         </is>
       </c>
     </row>
     <row r="276" ht="36" customHeight="1">
       <c r="A276" s="11" t="inlineStr">
         <is>
-          <t>IGRF000430006</t>
+          <t>IGRF000428000</t>
         </is>
       </c>
       <c r="B276" s="12" t="n">
@@ -19534,135 +19522,135 @@
       </c>
       <c r="C276" s="7" t="inlineStr">
         <is>
-          <t>TRITON Maximizer Dynamic Fund of Funds Class A</t>
+          <t>TRITON Maximizer Balanced Fund of Funds Class A</t>
         </is>
       </c>
       <c r="D276" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01029</t>
+          <t>EGRAK01030</t>
         </is>
       </c>
     </row>
     <row r="277" ht="36" customHeight="1">
       <c r="A277" s="13" t="inlineStr">
         <is>
-          <t>IGRF000432002</t>
+          <t>IGRF000430006</t>
         </is>
       </c>
       <c r="B277" s="14" t="n">
-        <v>45044</v>
+        <v>45021</v>
       </c>
       <c r="C277" s="5" t="inlineStr">
         <is>
-          <t>ALPHA Bancassurance EE105 Structured Fund</t>
+          <t>TRITON Maximizer Dynamic Fund of Funds Class A</t>
         </is>
       </c>
       <c r="D277" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01032</t>
+          <t>EGRAK01029</t>
         </is>
       </c>
     </row>
     <row r="278" ht="36" customHeight="1">
       <c r="A278" s="11" t="inlineStr">
         <is>
-          <t>IGRF000433000</t>
+          <t>IGRF000432002</t>
         </is>
       </c>
       <c r="B278" s="12" t="n">
-        <v>45058</v>
+        <v>45044</v>
       </c>
       <c r="C278" s="7" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME IV 5year - BOND FUND</t>
+          <t>ALPHA Bancassurance EE105 Structured Fund</t>
         </is>
       </c>
       <c r="D278" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01033</t>
+          <t>EGRAK01032</t>
         </is>
       </c>
     </row>
     <row r="279" ht="36" customHeight="1">
       <c r="A279" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01065_SHR</t>
+          <t>IGRF000433000</t>
         </is>
       </c>
       <c r="B279" s="14" t="n">
-        <v>45061</v>
-      </c>
-      <c r="C279" s="5" t="inlineStr"/>
+        <v>45058</v>
+      </c>
+      <c r="C279" s="5" t="inlineStr">
+        <is>
+          <t>DELOS EXTRA INCOME IV 5year - BOND FUND</t>
+        </is>
+      </c>
       <c r="D279" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01065</t>
+          <t>EGRAK01033</t>
         </is>
       </c>
     </row>
     <row r="280" ht="36" customHeight="1">
       <c r="A280" s="11" t="inlineStr">
         <is>
-          <t>IGRF000434008</t>
+          <t>PEGRAK01065_SHR</t>
         </is>
       </c>
       <c r="B280" s="12" t="n">
-        <v>45065</v>
-      </c>
-      <c r="C280" s="7" t="inlineStr">
-        <is>
-          <t>DELOS EXTRA INCOME USD 3year - BOND FUND</t>
-        </is>
-      </c>
+        <v>45061</v>
+      </c>
+      <c r="C280" s="7" t="inlineStr"/>
       <c r="D280" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01034</t>
+          <t>EGRAK01065</t>
         </is>
       </c>
     </row>
     <row r="281" ht="36" customHeight="1">
       <c r="A281" s="13" t="inlineStr">
         <is>
-          <t>IGRF000437001</t>
+          <t>IGRF000434008</t>
         </is>
       </c>
       <c r="B281" s="14" t="n">
-        <v>45070</v>
+        <v>45065</v>
       </c>
       <c r="C281" s="5" t="inlineStr">
         <is>
-          <t>EUROBANK GF TARGET MATURITY VI BOND FUND</t>
+          <t>DELOS EXTRA INCOME USD 3year - BOND FUND</t>
         </is>
       </c>
       <c r="D281" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01035</t>
+          <t>EGRAK01034</t>
         </is>
       </c>
     </row>
     <row r="282" ht="36" customHeight="1">
       <c r="A282" s="11" t="inlineStr">
         <is>
-          <t>IGRF000436003</t>
+          <t>IGRF000437001</t>
         </is>
       </c>
       <c r="B282" s="12" t="n">
-        <v>45078</v>
+        <v>45070</v>
       </c>
       <c r="C282" s="7" t="inlineStr">
         <is>
-          <t>Eurobank GF Target Maturity V Bond Fund</t>
+          <t>EUROBANK GF TARGET MATURITY VI BOND FUND</t>
         </is>
       </c>
       <c r="D282" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01038</t>
+          <t>EGRAK01035</t>
         </is>
       </c>
     </row>
     <row r="283" ht="36" customHeight="1">
       <c r="A283" s="13" t="inlineStr">
         <is>
-          <t>IGRF000441003</t>
+          <t>IGRF000436003</t>
         </is>
       </c>
       <c r="B283" s="14" t="n">
@@ -19670,39 +19658,39 @@
       </c>
       <c r="C283" s="5" t="inlineStr">
         <is>
-          <t>Eurobank GF Top 30 Select Structured Fund</t>
+          <t>Eurobank GF Target Maturity V Bond Fund</t>
         </is>
       </c>
       <c r="D283" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01037</t>
+          <t>EGRAK01038</t>
         </is>
       </c>
     </row>
     <row r="284" ht="36" customHeight="1">
       <c r="A284" s="11" t="inlineStr">
         <is>
-          <t>IGRF000439007</t>
+          <t>IGRF000441003</t>
         </is>
       </c>
       <c r="B284" s="12" t="n">
-        <v>45083</v>
+        <v>45078</v>
       </c>
       <c r="C284" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TARGET MATURITY III 2028 BOND FUND Classic D</t>
+          <t>Eurobank GF Top 30 Select Structured Fund</t>
         </is>
       </c>
       <c r="D284" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01041</t>
+          <t>EGRAK01037</t>
         </is>
       </c>
     </row>
     <row r="285" ht="36" customHeight="1">
       <c r="A285" s="13" t="inlineStr">
         <is>
-          <t>IGRF000440005</t>
+          <t>IGRF000439007</t>
         </is>
       </c>
       <c r="B285" s="14" t="n">
@@ -19710,383 +19698,383 @@
       </c>
       <c r="C285" s="5" t="inlineStr">
         <is>
-          <t>ALPHA MELLON II BALANCED FUND</t>
+          <t>ALPHA TARGET MATURITY III 2028 BOND FUND Classic D</t>
         </is>
       </c>
       <c r="D285" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01039</t>
+          <t>EGRAK01041</t>
         </is>
       </c>
     </row>
     <row r="286" ht="36" customHeight="1">
       <c r="A286" s="11" t="inlineStr">
         <is>
-          <t>IGRF000443009</t>
+          <t>IGRF000440005</t>
         </is>
       </c>
       <c r="B286" s="12" t="n">
-        <v>45089</v>
+        <v>45083</v>
       </c>
       <c r="C286" s="7" t="inlineStr">
         <is>
-          <t>Optima income bond fund</t>
+          <t>ALPHA MELLON II BALANCED FUND</t>
         </is>
       </c>
       <c r="D286" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01036</t>
+          <t>EGRAK01039</t>
         </is>
       </c>
     </row>
     <row r="287" ht="36" customHeight="1">
       <c r="A287" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01071_SHR</t>
+          <t>IGRF000443009</t>
         </is>
       </c>
       <c r="B287" s="14" t="n">
-        <v>45105</v>
-      </c>
-      <c r="C287" s="5" t="inlineStr"/>
+        <v>45089</v>
+      </c>
+      <c r="C287" s="5" t="inlineStr">
+        <is>
+          <t>Optima income bond fund</t>
+        </is>
+      </c>
       <c r="D287" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01071</t>
+          <t>EGRAK01036</t>
         </is>
       </c>
     </row>
     <row r="288" ht="36" customHeight="1">
       <c r="A288" s="11" t="inlineStr">
         <is>
-          <t>IGRF000448008</t>
+          <t>PEGRAK01071_SHR</t>
         </is>
       </c>
       <c r="B288" s="12" t="n">
-        <v>45110</v>
-      </c>
-      <c r="C288" s="7" t="inlineStr">
-        <is>
-          <t>DELOS EXTRA INCOME 18months - BOND FUND</t>
-        </is>
-      </c>
+        <v>45105</v>
+      </c>
+      <c r="C288" s="7" t="inlineStr"/>
       <c r="D288" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01040</t>
+          <t>EGRAK01071</t>
         </is>
       </c>
     </row>
     <row r="289" ht="36" customHeight="1">
       <c r="A289" s="13" t="inlineStr">
         <is>
-          <t>IGRF000447000</t>
+          <t>IGRF000448008</t>
         </is>
       </c>
       <c r="B289" s="14" t="n">
-        <v>45114</v>
+        <v>45110</v>
       </c>
       <c r="C289" s="5" t="inlineStr">
         <is>
-          <t>EUROBANK GF HELLAS INVEST DOMESTIC BALANCED FUND</t>
+          <t>DELOS EXTRA INCOME 18months - BOND FUND</t>
         </is>
       </c>
       <c r="D289" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01043</t>
+          <t>EGRAK01040</t>
         </is>
       </c>
     </row>
     <row r="290" ht="36" customHeight="1">
       <c r="A290" s="11" t="inlineStr">
         <is>
-          <t>PEGRAK01075_SHR</t>
+          <t>IGRF000447000</t>
         </is>
       </c>
       <c r="B290" s="12" t="n">
-        <v>45121</v>
-      </c>
-      <c r="C290" s="7" t="inlineStr"/>
+        <v>45114</v>
+      </c>
+      <c r="C290" s="7" t="inlineStr">
+        <is>
+          <t>EUROBANK GF HELLAS INVEST DOMESTIC BALANCED FUND</t>
+        </is>
+      </c>
       <c r="D290" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01075</t>
+          <t>EGRAK01043</t>
         </is>
       </c>
     </row>
     <row r="291" ht="36" customHeight="1">
       <c r="A291" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01074_SHR</t>
+          <t>PEGRAK01075_SHR</t>
         </is>
       </c>
       <c r="B291" s="14" t="n">
-        <v>45133</v>
+        <v>45121</v>
       </c>
       <c r="C291" s="5" t="inlineStr"/>
       <c r="D291" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01074</t>
+          <t>EGRAK01075</t>
         </is>
       </c>
     </row>
     <row r="292" ht="36" customHeight="1">
       <c r="A292" s="11" t="inlineStr">
         <is>
-          <t>IGRF000449006</t>
+          <t>PEGRAK01074_SHR</t>
         </is>
       </c>
       <c r="B292" s="12" t="n">
-        <v>45138</v>
-      </c>
-      <c r="C292" s="7" t="inlineStr">
-        <is>
-          <t>DELOS EXTRA INCOME V 5 years - Bond Fund</t>
-        </is>
-      </c>
+        <v>45133</v>
+      </c>
+      <c r="C292" s="7" t="inlineStr"/>
       <c r="D292" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01042</t>
+          <t>EGRAK01074</t>
         </is>
       </c>
     </row>
     <row r="293" ht="36" customHeight="1">
       <c r="A293" s="13" t="inlineStr">
         <is>
-          <t>IGRF000450004</t>
+          <t>IGRF000449006</t>
         </is>
       </c>
       <c r="B293" s="14" t="n">
-        <v>45146</v>
+        <v>45138</v>
       </c>
       <c r="C293" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2026 EUROPEAN BOND FUND</t>
+          <t>DELOS EXTRA INCOME V 5 years - Bond Fund</t>
         </is>
       </c>
       <c r="D293" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01044</t>
+          <t>EGRAK01042</t>
         </is>
       </c>
     </row>
     <row r="294" ht="36" customHeight="1">
       <c r="A294" s="11" t="inlineStr">
         <is>
-          <t>IGRF000451002</t>
+          <t>IGRF000450004</t>
         </is>
       </c>
       <c r="B294" s="12" t="n">
-        <v>45166</v>
+        <v>45146</v>
       </c>
       <c r="C294" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TARGET MATURITY IV 2028 BOND FUND CLASSIC</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2026 EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D294" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01045</t>
+          <t>EGRAK01044</t>
         </is>
       </c>
     </row>
     <row r="295" ht="36" customHeight="1">
       <c r="A295" s="13" t="inlineStr">
         <is>
-          <t>IGRF000454006</t>
+          <t>IGRF000451002</t>
         </is>
       </c>
       <c r="B295" s="14" t="n">
-        <v>45173</v>
+        <v>45166</v>
       </c>
       <c r="C295" s="5" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME II 18months - BOND FUND</t>
+          <t>ALPHA TARGET MATURITY IV 2028 BOND FUND CLASSIC</t>
         </is>
       </c>
       <c r="D295" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01049</t>
+          <t>EGRAK01045</t>
         </is>
       </c>
     </row>
     <row r="296" ht="36" customHeight="1">
       <c r="A296" s="11" t="inlineStr">
         <is>
-          <t>IGRF000453008</t>
+          <t>IGRF000454006</t>
         </is>
       </c>
       <c r="B296" s="12" t="n">
-        <v>45181</v>
+        <v>45173</v>
       </c>
       <c r="C296" s="7" t="inlineStr">
         <is>
-          <t>ALPHA Bancassurance EE106 Structured Fund</t>
+          <t>DELOS EXTRA INCOME II 18months - BOND FUND</t>
         </is>
       </c>
       <c r="D296" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01050</t>
+          <t>EGRAK01049</t>
         </is>
       </c>
     </row>
     <row r="297" ht="36" customHeight="1">
       <c r="A297" s="13" t="inlineStr">
         <is>
-          <t>IGRF000455003</t>
+          <t>IGRF000453008</t>
         </is>
       </c>
       <c r="B297" s="14" t="n">
-        <v>45187</v>
+        <v>45181</v>
       </c>
       <c r="C297" s="5" t="inlineStr">
         <is>
-          <t>3K/BANK OF ATTICA PREMIER INCOME BOND FUND</t>
+          <t>ALPHA Bancassurance EE106 Structured Fund</t>
         </is>
       </c>
       <c r="D297" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01047</t>
+          <t>EGRAK01050</t>
         </is>
       </c>
     </row>
     <row r="298" ht="36" customHeight="1">
       <c r="A298" s="11" t="inlineStr">
         <is>
-          <t>PEGRAK01076_SHR</t>
+          <t>IGRF000455003</t>
         </is>
       </c>
       <c r="B298" s="12" t="n">
-        <v>45219</v>
-      </c>
-      <c r="C298" s="7" t="inlineStr"/>
+        <v>45187</v>
+      </c>
+      <c r="C298" s="7" t="inlineStr">
+        <is>
+          <t>3K/BANK OF ATTICA PREMIER INCOME BOND FUND</t>
+        </is>
+      </c>
       <c r="D298" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01076</t>
+          <t>EGRAK01047</t>
         </is>
       </c>
     </row>
     <row r="299" ht="36" customHeight="1">
       <c r="A299" s="13" t="inlineStr">
         <is>
-          <t>IGRF000457009</t>
+          <t>PEGRAK01076_SHR</t>
         </is>
       </c>
       <c r="B299" s="14" t="n">
-        <v>45231</v>
-      </c>
-      <c r="C299" s="5" t="inlineStr">
-        <is>
-          <t>DELOS EXTRA INCOME 24months - BOND FUND</t>
-        </is>
-      </c>
+        <v>45219</v>
+      </c>
+      <c r="C299" s="5" t="inlineStr"/>
       <c r="D299" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01051</t>
+          <t>EGRAK01076</t>
         </is>
       </c>
     </row>
     <row r="300" ht="36" customHeight="1">
       <c r="A300" s="11" t="inlineStr">
         <is>
-          <t>IGRF000459005</t>
+          <t>IGRF000457009</t>
         </is>
       </c>
       <c r="B300" s="12" t="n">
-        <v>45236</v>
+        <v>45231</v>
       </c>
       <c r="C300" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TARGET MATURITY V 2028 BOND FUND CLASSIC D</t>
+          <t>DELOS EXTRA INCOME 24months - BOND FUND</t>
         </is>
       </c>
       <c r="D300" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01052</t>
+          <t>EGRAK01051</t>
         </is>
       </c>
     </row>
     <row r="301" ht="36" customHeight="1">
       <c r="A301" s="13" t="inlineStr">
         <is>
-          <t>IGRF000462009</t>
+          <t>IGRF000459005</t>
         </is>
       </c>
       <c r="B301" s="14" t="n">
-        <v>45252</v>
+        <v>45236</v>
       </c>
       <c r="C301" s="5" t="inlineStr">
         <is>
-          <t>GREEK FUND TARGET MATURITY VII BOND FUND - EUROBANK DIS CLASS</t>
+          <t>ALPHA TARGET MATURITY V 2028 BOND FUND CLASSIC D</t>
         </is>
       </c>
       <c r="D301" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01054</t>
+          <t>EGRAK01052</t>
         </is>
       </c>
     </row>
     <row r="302" ht="36" customHeight="1">
       <c r="A302" s="11" t="inlineStr">
         <is>
-          <t>IGRF000464005</t>
+          <t>IGRF000460003</t>
         </is>
       </c>
       <c r="B302" s="12" t="n">
-        <v>45268</v>
+        <v>45236</v>
       </c>
       <c r="C302" s="7" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME III 18months - BOND FUND</t>
+          <t>PIRAEUS INCOME 2025 EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D302" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01056</t>
+          <t>EGRAK01053</t>
         </is>
       </c>
     </row>
     <row r="303" ht="36" customHeight="1">
       <c r="A303" s="13" t="inlineStr">
         <is>
-          <t>IGRF000281003</t>
+          <t>IGRF000462009</t>
         </is>
       </c>
       <c r="B303" s="14" t="n">
-        <v>45274</v>
+        <v>45252</v>
       </c>
       <c r="C303" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS EUROPEAN BALANCED FUND (U)</t>
+          <t>GREEK FUND TARGET MATURITY VII BOND FUND - EUROBANK DIS CLASS</t>
         </is>
       </c>
       <c r="D303" s="5" t="inlineStr">
         <is>
-          <t>EGRAK00828</t>
+          <t>EGRAK01054</t>
         </is>
       </c>
     </row>
     <row r="304" ht="36" customHeight="1">
       <c r="A304" s="11" t="inlineStr">
         <is>
-          <t>IGRF000445004</t>
+          <t>IGRF000464005</t>
         </is>
       </c>
       <c r="B304" s="12" t="n">
-        <v>45274</v>
+        <v>45268</v>
       </c>
       <c r="C304" s="7" t="inlineStr">
         <is>
-          <t>PIRAEUS ESG EURO AGGREGATE BOND FUND (U)</t>
+          <t>DELOS EXTRA INCOME III 18months - BOND FUND</t>
         </is>
       </c>
       <c r="D304" s="7" t="inlineStr">
         <is>
-          <t>EGRAK00253</t>
+          <t>EGRAK01056</t>
         </is>
       </c>
     </row>
     <row r="305" ht="36" customHeight="1">
       <c r="A305" s="13" t="inlineStr">
         <is>
-          <t>IGRF000446002</t>
+          <t>IGRF000281003</t>
         </is>
       </c>
       <c r="B305" s="14" t="n">
@@ -20094,115 +20082,115 @@
       </c>
       <c r="C305" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS US EQUITY FUND (U)</t>
+          <t>PIRAEUS EUROPEAN BALANCED FUND (U)</t>
         </is>
       </c>
       <c r="D305" s="5" t="inlineStr">
         <is>
-          <t>EGRAK00512</t>
+          <t>EGRAK00828</t>
         </is>
       </c>
     </row>
     <row r="306" ht="36" customHeight="1">
       <c r="A306" s="11" t="inlineStr">
         <is>
-          <t>IGRF000466000</t>
+          <t>IGRF000445004</t>
         </is>
       </c>
       <c r="B306" s="12" t="n">
-        <v>45282</v>
+        <v>45274</v>
       </c>
       <c r="C306" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TARGET MATURITY VI 2026 BOND FUND Classic D</t>
+          <t>PIRAEUS ESG EURO AGGREGATE BOND FUND (U)</t>
         </is>
       </c>
       <c r="D306" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01055</t>
+          <t>EGRAK00253</t>
         </is>
       </c>
     </row>
     <row r="307" ht="36" customHeight="1">
       <c r="A307" s="13" t="inlineStr">
         <is>
-          <t>PEGRAEEAP012_SHR</t>
+          <t>IGRF000446002</t>
         </is>
       </c>
       <c r="B307" s="14" t="n">
-        <v>45287</v>
-      </c>
-      <c r="C307" s="5" t="inlineStr"/>
+        <v>45274</v>
+      </c>
+      <c r="C307" s="5" t="inlineStr">
+        <is>
+          <t>PIRAEUS US EQUITY FUND (U)</t>
+        </is>
+      </c>
       <c r="D307" s="5" t="inlineStr">
         <is>
-          <t>EGRAEEAP012</t>
+          <t>EGRAK00512</t>
         </is>
       </c>
     </row>
     <row r="308" ht="36" customHeight="1">
       <c r="A308" s="11" t="inlineStr">
         <is>
-          <t>IGRF000472008</t>
+          <t>IGRF000466000</t>
         </is>
       </c>
       <c r="B308" s="12" t="n">
-        <v>45307</v>
+        <v>45282</v>
       </c>
       <c r="C308" s="7" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME II 24months - BOND FUND</t>
+          <t>ALPHA TARGET MATURITY VI 2026 BOND FUND Classic D</t>
         </is>
       </c>
       <c r="D308" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01081</t>
+          <t>EGRAK01055</t>
         </is>
       </c>
     </row>
     <row r="309" ht="36" customHeight="1">
       <c r="A309" s="13" t="inlineStr">
         <is>
-          <t>IGRF000467008</t>
+          <t>PEGRAEEAP012_SHR</t>
         </is>
       </c>
       <c r="B309" s="14" t="n">
-        <v>45310</v>
-      </c>
-      <c r="C309" s="5" t="inlineStr">
-        <is>
-          <t>ALPHA Bancassurance EE107 Structured Fund</t>
-        </is>
-      </c>
+        <v>45287</v>
+      </c>
+      <c r="C309" s="5" t="inlineStr"/>
       <c r="D309" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01079</t>
+          <t>EGRAEEAP012</t>
         </is>
       </c>
     </row>
     <row r="310" ht="36" customHeight="1">
       <c r="A310" s="11" t="inlineStr">
         <is>
-          <t>IGRF000473006</t>
+          <t>IGRF000472008</t>
         </is>
       </c>
       <c r="B310" s="12" t="n">
-        <v>45310</v>
+        <v>45307</v>
       </c>
       <c r="C310" s="7" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2029 II EUROREAN BOND FUND</t>
+          <t>DELOS EXTRA INCOME II 24months - BOND FUND</t>
         </is>
       </c>
       <c r="D310" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01077</t>
+          <t>EGRAK01081</t>
         </is>
       </c>
     </row>
     <row r="311" ht="36" customHeight="1">
       <c r="A311" s="13" t="inlineStr">
         <is>
-          <t>IGRF000474004</t>
+          <t>IGRF000467008</t>
         </is>
       </c>
       <c r="B311" s="14" t="n">
@@ -20210,79 +20198,79 @@
       </c>
       <c r="C311" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS INCOME 2026 EUROPEAN BOND FUND</t>
+          <t>ALPHA Bancassurance EE107 Structured Fund</t>
         </is>
       </c>
       <c r="D311" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01078</t>
+          <t>EGRAK01079</t>
         </is>
       </c>
     </row>
     <row r="312" ht="36" customHeight="1">
       <c r="A312" s="11" t="inlineStr">
         <is>
-          <t>IGRF000471000</t>
+          <t>IGRF000473006</t>
         </is>
       </c>
       <c r="B312" s="12" t="n">
-        <v>45313</v>
+        <v>45310</v>
       </c>
       <c r="C312" s="7" t="inlineStr">
         <is>
-          <t>Optima income 2028 bond fund</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2029 II EUROREAN BOND FUND</t>
         </is>
       </c>
       <c r="D312" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01080</t>
+          <t>EGRAK01077</t>
         </is>
       </c>
     </row>
     <row r="313" ht="36" customHeight="1">
       <c r="A313" s="13" t="inlineStr">
         <is>
-          <t>IGRF000468006</t>
+          <t>IGRF000474004</t>
         </is>
       </c>
       <c r="B313" s="14" t="n">
-        <v>45327</v>
+        <v>45310</v>
       </c>
       <c r="C313" s="5" t="inlineStr">
         <is>
-          <t>ALPHA EURO SHORT-TERM BOND FUND Classic</t>
+          <t>PIRAEUS INCOME 2026 EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D313" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01082</t>
+          <t>EGRAK01078</t>
         </is>
       </c>
     </row>
     <row r="314" ht="36" customHeight="1">
       <c r="A314" s="11" t="inlineStr">
         <is>
-          <t>IGRF000469004</t>
+          <t>IGRF000471000</t>
         </is>
       </c>
       <c r="B314" s="12" t="n">
-        <v>45327</v>
+        <v>45313</v>
       </c>
       <c r="C314" s="7" t="inlineStr">
         <is>
-          <t>ALPHA EURO SHORT-TERM BOND FUND Classic D</t>
+          <t>Optima income 2028 bond fund</t>
         </is>
       </c>
       <c r="D314" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01082</t>
+          <t>EGRAK01080</t>
         </is>
       </c>
     </row>
     <row r="315" ht="36" customHeight="1">
       <c r="A315" s="13" t="inlineStr">
         <is>
-          <t>IGRF000470002</t>
+          <t>IGRF000468006</t>
         </is>
       </c>
       <c r="B315" s="14" t="n">
@@ -20290,7 +20278,7 @@
       </c>
       <c r="C315" s="5" t="inlineStr">
         <is>
-          <t>ALPHA EURO SHORT-TERM BOND FUND Institutional</t>
+          <t>ALPHA EURO SHORT-TERM BOND FUND Classic</t>
         </is>
       </c>
       <c r="D315" s="5" t="inlineStr">
@@ -20302,67 +20290,67 @@
     <row r="316" ht="36" customHeight="1">
       <c r="A316" s="11" t="inlineStr">
         <is>
-          <t>IGRF000482007</t>
+          <t>IGRF000469004</t>
         </is>
       </c>
       <c r="B316" s="12" t="n">
-        <v>45372</v>
+        <v>45327</v>
       </c>
       <c r="C316" s="7" t="inlineStr">
         <is>
-          <t>3K/BANK OF ATTICA PREMIER INCOME BOND FUND 2026</t>
+          <t>ALPHA EURO SHORT-TERM BOND FUND Classic D</t>
         </is>
       </c>
       <c r="D316" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01087</t>
+          <t>EGRAK01082</t>
         </is>
       </c>
     </row>
     <row r="317" ht="36" customHeight="1">
       <c r="A317" s="13" t="inlineStr">
         <is>
-          <t>IGRF000478005</t>
+          <t>IGRF000470002</t>
         </is>
       </c>
       <c r="B317" s="14" t="n">
-        <v>45377</v>
+        <v>45327</v>
       </c>
       <c r="C317" s="5" t="inlineStr">
         <is>
-          <t>NBG Asset Allocation Balanced - Balanced Fund of Funds</t>
+          <t>ALPHA EURO SHORT-TERM BOND FUND Institutional</t>
         </is>
       </c>
       <c r="D317" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01085</t>
+          <t>EGRAK01082</t>
         </is>
       </c>
     </row>
     <row r="318" ht="36" customHeight="1">
       <c r="A318" s="11" t="inlineStr">
         <is>
-          <t>IGRF000479003</t>
+          <t>IGRF000482007</t>
         </is>
       </c>
       <c r="B318" s="12" t="n">
-        <v>45377</v>
+        <v>45372</v>
       </c>
       <c r="C318" s="7" t="inlineStr">
         <is>
-          <t>NBG Asset Allocation Conservative -  Balanced Fund of Funds</t>
+          <t>3K/BANK OF ATTICA PREMIER INCOME BOND FUND 2026</t>
         </is>
       </c>
       <c r="D318" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01084</t>
+          <t>EGRAK01087</t>
         </is>
       </c>
     </row>
     <row r="319" ht="36" customHeight="1">
       <c r="A319" s="13" t="inlineStr">
         <is>
-          <t>IGRF000480001</t>
+          <t>IGRF000478005</t>
         </is>
       </c>
       <c r="B319" s="14" t="n">
@@ -20370,311 +20358,311 @@
       </c>
       <c r="C319" s="5" t="inlineStr">
         <is>
-          <t>NBG Asset Allocation Dynamic - Balanced Fund of Funds</t>
+          <t>NBG Asset Allocation Balanced - Balanced Fund of Funds</t>
         </is>
       </c>
       <c r="D319" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01086</t>
+          <t>EGRAK01085</t>
         </is>
       </c>
     </row>
     <row r="320" ht="36" customHeight="1">
       <c r="A320" s="11" t="inlineStr">
         <is>
-          <t>IGRF000477007</t>
+          <t>IGRF000479003</t>
         </is>
       </c>
       <c r="B320" s="12" t="n">
-        <v>45379</v>
+        <v>45377</v>
       </c>
       <c r="C320" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TARGET MATURITY VII 2026 BOND FUND CLASSIC D</t>
+          <t>NBG Asset Allocation Conservative -  Balanced Fund of Funds</t>
         </is>
       </c>
       <c r="D320" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01088</t>
+          <t>EGRAK01084</t>
         </is>
       </c>
     </row>
     <row r="321" ht="36" customHeight="1">
       <c r="A321" s="13" t="inlineStr">
         <is>
-          <t>IGRF000481009</t>
+          <t>IGRF000480001</t>
         </is>
       </c>
       <c r="B321" s="14" t="n">
-        <v>45379</v>
+        <v>45377</v>
       </c>
       <c r="C321" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2027 EUROREAN BOND FUND</t>
+          <t>NBG Asset Allocation Dynamic - Balanced Fund of Funds</t>
         </is>
       </c>
       <c r="D321" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01089</t>
+          <t>EGRAK01086</t>
         </is>
       </c>
     </row>
     <row r="322" ht="36" customHeight="1">
       <c r="A322" s="11" t="inlineStr">
         <is>
-          <t>IGRF000486008</t>
+          <t>IGRF000477007</t>
         </is>
       </c>
       <c r="B322" s="12" t="n">
-        <v>45397</v>
+        <v>45379</v>
       </c>
       <c r="C322" s="7" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME IV 24MONTHS - BOND FUND</t>
+          <t>ALPHA TARGET MATURITY VII 2026 BOND FUND CLASSIC D</t>
         </is>
       </c>
       <c r="D322" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01090</t>
+          <t>EGRAK01088</t>
         </is>
       </c>
     </row>
     <row r="323" ht="36" customHeight="1">
       <c r="A323" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01100_SHR</t>
+          <t>IGRF000481009</t>
         </is>
       </c>
       <c r="B323" s="14" t="n">
-        <v>45408</v>
-      </c>
-      <c r="C323" s="5" t="inlineStr"/>
+        <v>45379</v>
+      </c>
+      <c r="C323" s="5" t="inlineStr">
+        <is>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2027 EUROREAN BOND FUND</t>
+        </is>
+      </c>
       <c r="D323" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01100</t>
+          <t>EGRAK01089</t>
         </is>
       </c>
     </row>
     <row r="324" ht="36" customHeight="1">
       <c r="A324" s="11" t="inlineStr">
         <is>
-          <t>PEGRAK01099_SHR</t>
+          <t>IGRF000486008</t>
         </is>
       </c>
       <c r="B324" s="12" t="n">
-        <v>45411</v>
-      </c>
-      <c r="C324" s="7" t="inlineStr"/>
+        <v>45397</v>
+      </c>
+      <c r="C324" s="7" t="inlineStr">
+        <is>
+          <t>DELOS EXTRA INCOME IV 24MONTHS - BOND FUND</t>
+        </is>
+      </c>
       <c r="D324" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01099</t>
+          <t>EGRAK01090</t>
         </is>
       </c>
     </row>
     <row r="325" ht="36" customHeight="1">
       <c r="A325" s="13" t="inlineStr">
         <is>
-          <t>IGRF000487006</t>
+          <t>PEGRAK01100_SHR</t>
         </is>
       </c>
       <c r="B325" s="14" t="n">
-        <v>45412</v>
-      </c>
-      <c r="C325" s="5" t="inlineStr">
-        <is>
-          <t>Piraeus Income 2026 (II) European Bond Fund</t>
-        </is>
-      </c>
+        <v>45408</v>
+      </c>
+      <c r="C325" s="5" t="inlineStr"/>
       <c r="D325" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01091</t>
+          <t>EGRAK01100</t>
         </is>
       </c>
     </row>
     <row r="326" ht="36" customHeight="1">
       <c r="A326" s="11" t="inlineStr">
         <is>
-          <t>IGRF000490000</t>
+          <t>PEGRAK01099_SHR</t>
         </is>
       </c>
       <c r="B326" s="12" t="n">
-        <v>45422</v>
-      </c>
-      <c r="C326" s="7" t="inlineStr">
-        <is>
-          <t>OPTIMA INCOME 2029 BOND FUND</t>
-        </is>
-      </c>
+        <v>45411</v>
+      </c>
+      <c r="C326" s="7" t="inlineStr"/>
       <c r="D326" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01092</t>
+          <t>EGRAK01099</t>
         </is>
       </c>
     </row>
     <row r="327" ht="36" customHeight="1">
       <c r="A327" s="13" t="inlineStr">
         <is>
-          <t>IGRF000489002</t>
+          <t>IGRF000487006</t>
         </is>
       </c>
       <c r="B327" s="14" t="n">
-        <v>45442</v>
+        <v>45412</v>
       </c>
       <c r="C327" s="5" t="inlineStr">
         <is>
-          <t>ALPHA BANCASSURANCE EE108 STRUCTURED FUND</t>
+          <t>Piraeus Income 2026 (II) European Bond Fund</t>
         </is>
       </c>
       <c r="D327" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01093</t>
+          <t>EGRAK01091</t>
         </is>
       </c>
     </row>
     <row r="328" ht="36" customHeight="1">
       <c r="A328" s="11" t="inlineStr">
         <is>
-          <t>IGRF000491008</t>
+          <t>IGRF000490000</t>
         </is>
       </c>
       <c r="B328" s="12" t="n">
-        <v>45446</v>
+        <v>45422</v>
       </c>
       <c r="C328" s="7" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME V 24MONTHS - BOND FUND</t>
+          <t>OPTIMA INCOME 2029 BOND FUND</t>
         </is>
       </c>
       <c r="D328" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01094</t>
+          <t>EGRAK01092</t>
         </is>
       </c>
     </row>
     <row r="329" ht="36" customHeight="1">
       <c r="A329" s="13" t="inlineStr">
         <is>
-          <t>IGRF000492006</t>
+          <t>IGRF000489002</t>
         </is>
       </c>
       <c r="B329" s="14" t="n">
-        <v>45492</v>
+        <v>45442</v>
       </c>
       <c r="C329" s="5" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME VI 24MONTHS - BOND FUND</t>
+          <t>ALPHA BANCASSURANCE EE108 STRUCTURED FUND</t>
         </is>
       </c>
       <c r="D329" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01095</t>
+          <t>EGRAK01093</t>
         </is>
       </c>
     </row>
     <row r="330" ht="36" customHeight="1">
       <c r="A330" s="11" t="inlineStr">
         <is>
-          <t>PEGRAK01102_SHR</t>
+          <t>IGRF000491008</t>
         </is>
       </c>
       <c r="B330" s="12" t="n">
-        <v>45496</v>
-      </c>
-      <c r="C330" s="7" t="inlineStr"/>
+        <v>45446</v>
+      </c>
+      <c r="C330" s="7" t="inlineStr">
+        <is>
+          <t>DELOS EXTRA INCOME V 24MONTHS - BOND FUND</t>
+        </is>
+      </c>
       <c r="D330" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01102</t>
+          <t>EGRAK01094</t>
         </is>
       </c>
     </row>
     <row r="331" ht="36" customHeight="1">
       <c r="A331" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01104_SHR</t>
+          <t>IGRF000492006</t>
         </is>
       </c>
       <c r="B331" s="14" t="n">
-        <v>45502</v>
-      </c>
-      <c r="C331" s="5" t="inlineStr"/>
+        <v>45492</v>
+      </c>
+      <c r="C331" s="5" t="inlineStr">
+        <is>
+          <t>DELOS EXTRA INCOME VI 24MONTHS - BOND FUND</t>
+        </is>
+      </c>
       <c r="D331" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01104</t>
+          <t>EGRAK01095</t>
         </is>
       </c>
     </row>
     <row r="332" ht="36" customHeight="1">
       <c r="A332" s="11" t="inlineStr">
         <is>
-          <t>IGRF000493004</t>
+          <t>PEGRAK01102_SHR</t>
         </is>
       </c>
       <c r="B332" s="12" t="n">
-        <v>45504</v>
-      </c>
-      <c r="C332" s="7" t="inlineStr">
-        <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2027 (II) EUROPEAN BOND FUND</t>
-        </is>
-      </c>
+        <v>45496</v>
+      </c>
+      <c r="C332" s="7" t="inlineStr"/>
       <c r="D332" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01096</t>
+          <t>EGRAK01102</t>
         </is>
       </c>
     </row>
     <row r="333" ht="36" customHeight="1">
       <c r="A333" s="13" t="inlineStr">
         <is>
-          <t>IGRF000495009</t>
+          <t>PEGRAK01104_SHR</t>
         </is>
       </c>
       <c r="B333" s="14" t="n">
-        <v>45513</v>
-      </c>
-      <c r="C333" s="5" t="inlineStr">
-        <is>
-          <t>TRITON Target Maturity Class A</t>
-        </is>
-      </c>
+        <v>45502</v>
+      </c>
+      <c r="C333" s="5" t="inlineStr"/>
       <c r="D333" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01097</t>
+          <t>EGRAK01104</t>
         </is>
       </c>
     </row>
     <row r="334" ht="36" customHeight="1">
       <c r="A334" s="11" t="inlineStr">
         <is>
-          <t>IGRF000494002</t>
+          <t>IGRF000493004</t>
         </is>
       </c>
       <c r="B334" s="12" t="n">
-        <v>45546</v>
+        <v>45504</v>
       </c>
       <c r="C334" s="7" t="inlineStr">
         <is>
-          <t>PIRAEUS IDEAS GLOBAL EQUITY FUND (R)</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2027 (II) EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D334" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01004</t>
+          <t>EGRAK01096</t>
         </is>
       </c>
     </row>
     <row r="335" ht="36" customHeight="1">
       <c r="A335" s="13" t="inlineStr">
         <is>
-          <t>IGRF000496007</t>
+          <t>IGRF000495009</t>
         </is>
       </c>
       <c r="B335" s="14" t="n">
-        <v>45547</v>
+        <v>45513</v>
       </c>
       <c r="C335" s="5" t="inlineStr">
         <is>
-          <t>TRITON Target Maturity Class E</t>
+          <t>TRITON Target Maturity Class A</t>
         </is>
       </c>
       <c r="D335" s="5" t="inlineStr">
@@ -20686,243 +20674,243 @@
     <row r="336" ht="36" customHeight="1">
       <c r="A336" s="11" t="inlineStr">
         <is>
-          <t>IGRF000497005</t>
+          <t>IGRF000494002</t>
         </is>
       </c>
       <c r="B336" s="12" t="n">
-        <v>45551</v>
+        <v>45546</v>
       </c>
       <c r="C336" s="7" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME VII 24MONTHS - BOND FUND</t>
+          <t>PIRAEUS IDEAS GLOBAL EQUITY FUND (R)</t>
         </is>
       </c>
       <c r="D336" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01098</t>
+          <t>EGRAK01004</t>
         </is>
       </c>
     </row>
     <row r="337" ht="36" customHeight="1">
       <c r="A337" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01103_SHR</t>
+          <t>IGRF000496007</t>
         </is>
       </c>
       <c r="B337" s="14" t="n">
-        <v>45552</v>
-      </c>
-      <c r="C337" s="5" t="inlineStr"/>
+        <v>45547</v>
+      </c>
+      <c r="C337" s="5" t="inlineStr">
+        <is>
+          <t>TRITON Target Maturity Class E</t>
+        </is>
+      </c>
       <c r="D337" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01103</t>
+          <t>EGRAK01097</t>
         </is>
       </c>
     </row>
     <row r="338" ht="36" customHeight="1">
       <c r="A338" s="11" t="inlineStr">
         <is>
-          <t>PEGRAK01127_SHR</t>
+          <t>IGRF000497005</t>
         </is>
       </c>
       <c r="B338" s="12" t="n">
-        <v>45562</v>
+        <v>45551</v>
       </c>
       <c r="C338" s="7" t="inlineStr">
         <is>
-          <t>SUSTAINABLE FORWARD CAPITAL FUND I AKES</t>
+          <t>DELOS EXTRA INCOME VII 24MONTHS - BOND FUND</t>
         </is>
       </c>
       <c r="D338" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01127</t>
+          <t>EGRAK01098</t>
         </is>
       </c>
     </row>
     <row r="339" ht="36" customHeight="1">
       <c r="A339" s="13" t="inlineStr">
         <is>
-          <t>IGRF000504008</t>
+          <t>PEGRAK01103_SHR</t>
         </is>
       </c>
       <c r="B339" s="14" t="n">
-        <v>45572</v>
-      </c>
-      <c r="C339" s="5" t="inlineStr">
-        <is>
-          <t>OPTIMA INCOME 2026 BOND FUND</t>
-        </is>
-      </c>
+        <v>45552</v>
+      </c>
+      <c r="C339" s="5" t="inlineStr"/>
       <c r="D339" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01107</t>
+          <t>EGRAK01103</t>
         </is>
       </c>
     </row>
     <row r="340" ht="36" customHeight="1">
       <c r="A340" s="11" t="inlineStr">
         <is>
-          <t>IGRF000499001</t>
+          <t>PEGRAK01127_SHR</t>
         </is>
       </c>
       <c r="B340" s="12" t="n">
-        <v>45576</v>
+        <v>45562</v>
       </c>
       <c r="C340" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TARGET MATURITY VIII 2029 BOND FUND CLASSIC D</t>
+          <t>SUSTAINABLE FORWARD CAPITAL FUND I AKES</t>
         </is>
       </c>
       <c r="D340" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01105</t>
+          <t>EGRAK01127</t>
         </is>
       </c>
     </row>
     <row r="341" ht="36" customHeight="1">
       <c r="A341" s="13" t="inlineStr">
         <is>
-          <t>IGRF000501004</t>
+          <t>IGRF000504008</t>
         </is>
       </c>
       <c r="B341" s="14" t="n">
-        <v>45576</v>
+        <v>45572</v>
       </c>
       <c r="C341" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2029 (III) EUROPEAN BOND FUND</t>
+          <t>OPTIMA INCOME 2026 BOND FUND</t>
         </is>
       </c>
       <c r="D341" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01101</t>
+          <t>EGRAK01107</t>
         </is>
       </c>
     </row>
     <row r="342" ht="36" customHeight="1">
       <c r="A342" s="11" t="inlineStr">
         <is>
-          <t>IGRF000500006</t>
+          <t>IGRF000499001</t>
         </is>
       </c>
       <c r="B342" s="12" t="n">
-        <v>45586</v>
+        <v>45576</v>
       </c>
       <c r="C342" s="7" t="inlineStr">
         <is>
-          <t>ALPHA BANCASSURANCE EE109 STRUCTURED FUND</t>
+          <t>ALPHA TARGET MATURITY VIII 2029 BOND FUND CLASSIC D</t>
         </is>
       </c>
       <c r="D342" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01106</t>
+          <t>EGRAK01105</t>
         </is>
       </c>
     </row>
     <row r="343" ht="36" customHeight="1">
       <c r="A343" s="13" t="inlineStr">
         <is>
-          <t>PEGRAK01128_SHR</t>
+          <t>IGRF000501004</t>
         </is>
       </c>
       <c r="B343" s="14" t="n">
-        <v>45604</v>
+        <v>45576</v>
       </c>
       <c r="C343" s="5" t="inlineStr">
         <is>
-          <t>EVERCURIOUS FUND I A.K.E.S.</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2029 (III) EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D343" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01128</t>
+          <t>EGRAK01101</t>
         </is>
       </c>
     </row>
     <row r="344" ht="36" customHeight="1">
       <c r="A344" s="11" t="inlineStr">
         <is>
-          <t>IGRF000507001</t>
+          <t>IGRF000500006</t>
         </is>
       </c>
       <c r="B344" s="12" t="n">
-        <v>45642</v>
+        <v>45586</v>
       </c>
       <c r="C344" s="7" t="inlineStr">
         <is>
-          <t>ALPHA TRUST APOLLO 11 GREEK EQUITY FUND</t>
+          <t>ALPHA BANCASSURANCE EE109 STRUCTURED FUND</t>
         </is>
       </c>
       <c r="D344" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01110</t>
+          <t>EGRAK01106</t>
         </is>
       </c>
     </row>
     <row r="345" ht="36" customHeight="1">
       <c r="A345" s="13" t="inlineStr">
         <is>
-          <t>IGRF000508009</t>
+          <t>PEGRAK01128_SHR</t>
         </is>
       </c>
       <c r="B345" s="14" t="n">
-        <v>45642</v>
+        <v>45604</v>
       </c>
       <c r="C345" s="5" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME IX 24MONTHS - BOND FUND</t>
+          <t>EVERCURIOUS FUND I A.K.E.S.</t>
         </is>
       </c>
       <c r="D345" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01111</t>
+          <t>EGRAK01128</t>
         </is>
       </c>
     </row>
     <row r="346" ht="36" customHeight="1">
       <c r="A346" s="11" t="inlineStr">
         <is>
-          <t>IGRF000509007</t>
+          <t>IGRF000507001</t>
         </is>
       </c>
       <c r="B346" s="12" t="n">
-        <v>45653</v>
+        <v>45642</v>
       </c>
       <c r="C346" s="7" t="inlineStr">
         <is>
-          <t>ATHOS - KM Cube - SkyNet US Equities Fund (Class A)</t>
+          <t>ALPHA TRUST APOLLO 11 GREEK EQUITY FUND</t>
         </is>
       </c>
       <c r="D346" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01112</t>
+          <t>EGRAK01110</t>
         </is>
       </c>
     </row>
     <row r="347" ht="36" customHeight="1">
       <c r="A347" s="13" t="inlineStr">
         <is>
-          <t>IGRF000510005</t>
+          <t>IGRF000508009</t>
         </is>
       </c>
       <c r="B347" s="14" t="n">
-        <v>45653</v>
+        <v>45642</v>
       </c>
       <c r="C347" s="5" t="inlineStr">
         <is>
-          <t>ATHOS - KM Cube - SkyNet US Equities Fund (Class B)</t>
+          <t>DELOS EXTRA INCOME IX 24MONTHS - BOND FUND</t>
         </is>
       </c>
       <c r="D347" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01112</t>
+          <t>EGRAK01111</t>
         </is>
       </c>
     </row>
     <row r="348" ht="36" customHeight="1">
       <c r="A348" s="11" t="inlineStr">
         <is>
-          <t>IGRF000511003</t>
+          <t>IGRF000509007</t>
         </is>
       </c>
       <c r="B348" s="12" t="n">
@@ -20930,7 +20918,7 @@
       </c>
       <c r="C348" s="7" t="inlineStr">
         <is>
-          <t>ATHOS - KM Cube - SkyNet US Equities Fund (Class I)</t>
+          <t>ATHOS - KM Cube - SkyNet US Equities Fund (Class A)</t>
         </is>
       </c>
       <c r="D348" s="7" t="inlineStr">
@@ -20942,7 +20930,7 @@
     <row r="349" ht="36" customHeight="1">
       <c r="A349" s="13" t="inlineStr">
         <is>
-          <t>IGRF000512001</t>
+          <t>IGRF000510005</t>
         </is>
       </c>
       <c r="B349" s="14" t="n">
@@ -20950,7 +20938,7 @@
       </c>
       <c r="C349" s="5" t="inlineStr">
         <is>
-          <t>ATHOS - KM Cube - SkyNet US Equities Fund (Class E-USD)</t>
+          <t>ATHOS - KM Cube - SkyNet US Equities Fund (Class B)</t>
         </is>
       </c>
       <c r="D349" s="5" t="inlineStr">
@@ -20962,107 +20950,107 @@
     <row r="350" ht="36" customHeight="1">
       <c r="A350" s="11" t="inlineStr">
         <is>
-          <t>IGRF000514007</t>
+          <t>IGRF000511003</t>
         </is>
       </c>
       <c r="B350" s="12" t="n">
-        <v>45671</v>
+        <v>45653</v>
       </c>
       <c r="C350" s="7" t="inlineStr">
         <is>
-          <t>PIRAEUS REGULAR INCOME STRATEGY 2028 (III) EUROPEAN BOND FUND</t>
+          <t>ATHOS - KM Cube - SkyNet US Equities Fund (Class I)</t>
         </is>
       </c>
       <c r="D350" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01113</t>
+          <t>EGRAK01112</t>
         </is>
       </c>
     </row>
     <row r="351" ht="36" customHeight="1">
       <c r="A351" s="13" t="inlineStr">
         <is>
-          <t>IGRF000513009</t>
+          <t>IGRF000512001</t>
         </is>
       </c>
       <c r="B351" s="14" t="n">
-        <v>45679</v>
+        <v>45653</v>
       </c>
       <c r="C351" s="5" t="inlineStr">
         <is>
-          <t>OPTIMA INCOME 2030 BOND FUND</t>
+          <t>ATHOS - KM Cube - SkyNet US Equities Fund (Class E-USD)</t>
         </is>
       </c>
       <c r="D351" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01114</t>
+          <t>EGRAK01112</t>
         </is>
       </c>
     </row>
     <row r="352" ht="36" customHeight="1">
       <c r="A352" s="11" t="inlineStr">
         <is>
-          <t>PEGRAK01129_SHR</t>
+          <t>IGRF000514007</t>
         </is>
       </c>
       <c r="B352" s="12" t="n">
-        <v>45679</v>
+        <v>45671</v>
       </c>
       <c r="C352" s="7" t="inlineStr">
         <is>
-          <t>GOLDEN AGE FUND I A.K.E.S</t>
+          <t>PIRAEUS REGULAR INCOME STRATEGY 2028 (III) EUROPEAN BOND FUND</t>
         </is>
       </c>
       <c r="D352" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01129</t>
+          <t>EGRAK01113</t>
         </is>
       </c>
     </row>
     <row r="353" ht="36" customHeight="1">
       <c r="A353" s="13" t="inlineStr">
         <is>
-          <t>IGRF000515004</t>
+          <t>IGRF000513009</t>
         </is>
       </c>
       <c r="B353" s="14" t="n">
-        <v>45681</v>
+        <v>45679</v>
       </c>
       <c r="C353" s="5" t="inlineStr">
         <is>
-          <t>ALPHA PROSPERITY II 90-130 STRUCTURED FUND</t>
+          <t>OPTIMA INCOME 2030 BOND FUND</t>
         </is>
       </c>
       <c r="D353" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01115</t>
+          <t>EGRAK01114</t>
         </is>
       </c>
     </row>
     <row r="354" ht="36" customHeight="1">
       <c r="A354" s="11" t="inlineStr">
         <is>
-          <t>IGRF000516002</t>
+          <t>PEGRAK01129_SHR</t>
         </is>
       </c>
       <c r="B354" s="12" t="n">
-        <v>45681</v>
+        <v>45679</v>
       </c>
       <c r="C354" s="7" t="inlineStr">
         <is>
-          <t>ALPHA GREEK EQUITY QUALITY INCOME FUND CLASSIC</t>
+          <t>GOLDEN AGE FUND I A.K.E.S</t>
         </is>
       </c>
       <c r="D354" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01116</t>
+          <t>EGRAK01129</t>
         </is>
       </c>
     </row>
     <row r="355" ht="36" customHeight="1">
       <c r="A355" s="13" t="inlineStr">
         <is>
-          <t>IGRF000517000</t>
+          <t>IGRF000515004</t>
         </is>
       </c>
       <c r="B355" s="14" t="n">
@@ -21070,19 +21058,19 @@
       </c>
       <c r="C355" s="5" t="inlineStr">
         <is>
-          <t>ALPHA GREEK EQUITY QUALITY INCOME FUND INSTITUTIONAL</t>
+          <t>ALPHA PROSPERITY II 90-130 STRUCTURED FUND</t>
         </is>
       </c>
       <c r="D355" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01116</t>
+          <t>EGRAK01115</t>
         </is>
       </c>
     </row>
     <row r="356" ht="36" customHeight="1">
       <c r="A356" s="11" t="inlineStr">
         <is>
-          <t>IGRF000518008</t>
+          <t>IGRF000516002</t>
         </is>
       </c>
       <c r="B356" s="12" t="n">
@@ -21090,7 +21078,7 @@
       </c>
       <c r="C356" s="7" t="inlineStr">
         <is>
-          <t>ALPHA GREEK EQUITY QUALITY INCOME FUND CLASSIC D</t>
+          <t>ALPHA GREEK EQUITY QUALITY INCOME FUND CLASSIC</t>
         </is>
       </c>
       <c r="D356" s="7" t="inlineStr">
@@ -21102,125 +21090,145 @@
     <row r="357" ht="36" customHeight="1">
       <c r="A357" s="13" t="inlineStr">
         <is>
-          <t>IGRF000520004</t>
+          <t>IGRF000517000</t>
         </is>
       </c>
       <c r="B357" s="14" t="n">
-        <v>45693</v>
+        <v>45681</v>
       </c>
       <c r="C357" s="5" t="inlineStr">
         <is>
-          <t>PIRAEUS ENHANCED INCOME BOND FUND</t>
+          <t>ALPHA GREEK EQUITY QUALITY INCOME FUND INSTITUTIONAL</t>
         </is>
       </c>
       <c r="D357" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01117</t>
+          <t>EGRAK01116</t>
         </is>
       </c>
     </row>
     <row r="358" ht="36" customHeight="1">
       <c r="A358" s="11" t="inlineStr">
         <is>
-          <t>IGRF000519006</t>
+          <t>IGRF000518008</t>
         </is>
       </c>
       <c r="B358" s="12" t="n">
-        <v>45698</v>
+        <v>45681</v>
       </c>
       <c r="C358" s="7" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME X 24MONTHS - BOND FUND</t>
+          <t>ALPHA GREEK EQUITY QUALITY INCOME FUND CLASSIC D</t>
         </is>
       </c>
       <c r="D358" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01118</t>
+          <t>EGRAK01116</t>
         </is>
       </c>
     </row>
     <row r="359" ht="36" customHeight="1">
       <c r="A359" s="13" t="inlineStr">
         <is>
-          <t>IGRF000522000</t>
+          <t>IGRF000520004</t>
         </is>
       </c>
       <c r="B359" s="14" t="n">
-        <v>45716</v>
+        <v>45693</v>
       </c>
       <c r="C359" s="5" t="inlineStr">
         <is>
-          <t>ALPHA Bancassurance EE110 Structured Fund</t>
+          <t>PIRAEUS ENHANCED INCOME BOND FUND</t>
         </is>
       </c>
       <c r="D359" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01119</t>
+          <t>EGRAK01117</t>
         </is>
       </c>
     </row>
     <row r="360" ht="36" customHeight="1">
       <c r="A360" s="11" t="inlineStr">
         <is>
-          <t>IGRF000521002</t>
+          <t>IGRF000519006</t>
         </is>
       </c>
       <c r="B360" s="12" t="n">
-        <v>45720</v>
+        <v>45698</v>
       </c>
       <c r="C360" s="7" t="inlineStr">
         <is>
-          <t>Optima income 2030 II bond fund</t>
+          <t>DELOS EXTRA INCOME X 24MONTHS - BOND FUND</t>
         </is>
       </c>
       <c r="D360" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01120</t>
+          <t>EGRAK01118</t>
         </is>
       </c>
     </row>
     <row r="361" ht="36" customHeight="1">
       <c r="A361" s="13" t="inlineStr">
         <is>
-          <t>IGRF000523008</t>
+          <t>IGRF000522000</t>
         </is>
       </c>
       <c r="B361" s="14" t="n">
-        <v>45733</v>
+        <v>45716</v>
       </c>
       <c r="C361" s="5" t="inlineStr">
         <is>
-          <t>DELOS EXTRA INCOME XI 24months - BOND FUND</t>
+          <t>ALPHA Bancassurance EE110 Structured Fund</t>
         </is>
       </c>
       <c r="D361" s="5" t="inlineStr">
         <is>
-          <t>EGRAK01121</t>
+          <t>EGRAK01119</t>
         </is>
       </c>
     </row>
     <row r="362" ht="36" customHeight="1">
       <c r="A362" s="11" t="inlineStr">
         <is>
-          <t>IGRF000460003</t>
+          <t>IGRF000521002</t>
         </is>
       </c>
       <c r="B362" s="12" t="n">
-        <v>45747</v>
+        <v>45720</v>
       </c>
       <c r="C362" s="7" t="inlineStr">
         <is>
-          <t>PIRAEUS INCOME 2027 EUROPEAN BOND FUND</t>
+          <t>Optima income 2030 II bond fund</t>
         </is>
       </c>
       <c r="D362" s="7" t="inlineStr">
         <is>
-          <t>EGRAK01053, EGRAK01122</t>
+          <t>EGRAK01120</t>
+        </is>
+      </c>
+    </row>
+    <row r="363" ht="36" customHeight="1">
+      <c r="A363" s="13" t="inlineStr">
+        <is>
+          <t>IGRF000523008</t>
+        </is>
+      </c>
+      <c r="B363" s="14" t="n">
+        <v>45733</v>
+      </c>
+      <c r="C363" s="5" t="inlineStr">
+        <is>
+          <t>DELOS EXTRA INCOME XI 24months - BOND FUND</t>
+        </is>
+      </c>
+      <c r="D363" s="5" t="inlineStr">
+        <is>
+          <t>EGRAK01121</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D362"/>
+  <autoFilter ref="A1:D363"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>